<commit_message>
Add mutational signatures table
</commit_message>
<xml_diff>
--- a/tables/mutational_signatures.xlsx
+++ b/tables/mutational_signatures.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="135">
   <si>
     <t xml:space="preserve">patient_id</t>
   </si>
@@ -294,6 +294,9 @@
     <t xml:space="preserve">SPECTRUM-OV-123</t>
   </si>
   <si>
+    <t xml:space="preserve">topic</t>
+  </si>
+  <si>
     <t xml:space="preserve">063</t>
   </si>
   <si>
@@ -361,6 +364,60 @@
   </si>
   <si>
     <t xml:space="preserve">083</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBS5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBS8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBS40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POLH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MMRD1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MMRD2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APOBEC1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APOBEC2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S-Dup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M-Dup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L-Dup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S-Del</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L-Del</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clust-FBI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clust-SV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FBI/Inv</t>
   </si>
 </sst>
 </file>
@@ -1794,1353 +1851,1413 @@
       <c r="W1" t="s">
         <v>115</v>
       </c>
+      <c r="X1" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" t="n">
         <v>0.55867102797821</v>
       </c>
-      <c r="B2" t="n">
+      <c r="C2" t="n">
         <v>0.653823517920692</v>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>-0.337416099799313</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>-0.379195664522017</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>-0.388345311851232</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>-0.370290032650612</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>-0.405740686540713</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>-0.416759970706528</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>-0.314890984850368</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>-0.175396651095867</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>-0.379036366438699</v>
       </c>
-      <c r="L2" t="n">
+      <c r="M2" t="n">
         <v>0.614015866517648</v>
       </c>
-      <c r="M2" t="n">
+      <c r="N2" t="n">
         <v>-0.375890809350173</v>
       </c>
-      <c r="N2" t="n">
+      <c r="O2" t="n">
         <v>-0.367534703000738</v>
       </c>
-      <c r="O2" t="n">
+      <c r="P2" t="n">
         <v>-0.414438563432522</v>
       </c>
-      <c r="P2" t="n">
+      <c r="Q2" t="n">
         <v>-0.406328020619258</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="R2" t="n">
         <v>-0.329107086311861</v>
       </c>
-      <c r="R2" t="n">
+      <c r="S2" t="n">
         <v>-0.131914228789296</v>
       </c>
-      <c r="S2" t="n">
+      <c r="T2" t="n">
         <v>-0.402455942894852</v>
       </c>
-      <c r="T2" t="n">
+      <c r="U2" t="n">
         <v>0.968983406002764</v>
       </c>
-      <c r="U2" t="n">
+      <c r="V2" t="n">
         <v>-0.420263278255262</v>
       </c>
-      <c r="V2" t="n">
+      <c r="W2" t="n">
         <v>-0.372989391074907</v>
       </c>
-      <c r="W2" t="n">
+      <c r="X2" t="n">
         <v>0.00259478318362204</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" t="n">
         <v>1.46191212775567</v>
       </c>
-      <c r="B3" t="n">
+      <c r="C3" t="n">
         <v>1.6547219708436</v>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>-0.220232635929218</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>-0.130100551073815</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>-0.678610977143744</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>-0.951604850227953</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>-0.668449087733363</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>-0.736920201729118</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>-0.0708186380420548</v>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>0.806671746342279</v>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
         <v>-0.418923448549546</v>
       </c>
-      <c r="L3" t="n">
+      <c r="M3" t="n">
         <v>1.39014296970378</v>
       </c>
-      <c r="M3" t="n">
+      <c r="N3" t="n">
         <v>-0.488634396625447</v>
       </c>
-      <c r="N3" t="n">
+      <c r="O3" t="n">
         <v>-0.619971191470381</v>
       </c>
-      <c r="O3" t="n">
+      <c r="P3" t="n">
         <v>-1.04747641165838</v>
       </c>
-      <c r="P3" t="n">
+      <c r="Q3" t="n">
         <v>-1.47901635168261</v>
       </c>
-      <c r="Q3" t="n">
+      <c r="R3" t="n">
         <v>-0.119059635480957</v>
       </c>
-      <c r="R3" t="n">
+      <c r="S3" t="n">
         <v>0.346192879547475</v>
       </c>
-      <c r="S3" t="n">
+      <c r="T3" t="n">
         <v>-0.714966854199836</v>
       </c>
-      <c r="T3" t="n">
+      <c r="U3" t="n">
         <v>1.10722548840639</v>
       </c>
-      <c r="U3" t="n">
+      <c r="V3" t="n">
         <v>-1.07274884302543</v>
       </c>
-      <c r="V3" t="n">
+      <c r="W3" t="n">
         <v>0.0832116334155547</v>
       </c>
-      <c r="W3" t="n">
+      <c r="X3" t="n">
         <v>0.909407102059476</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B4" t="n">
         <v>-0.986761390406177</v>
       </c>
-      <c r="B4" t="n">
+      <c r="C4" t="n">
         <v>-0.772044012093793</v>
       </c>
-      <c r="C4" t="n">
+      <c r="D4" t="n">
         <v>0.974089981270711</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>1.05135302009463</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>1.604593177777</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>0.576975787416958</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>1.29165471031182</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>1.51657931504448</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>0.561867379264542</v>
       </c>
-      <c r="J4" t="n">
+      <c r="K4" t="n">
         <v>-0.0814312049293967</v>
       </c>
-      <c r="K4" t="n">
+      <c r="L4" t="n">
         <v>1.1713407657516</v>
       </c>
-      <c r="L4" t="n">
+      <c r="M4" t="n">
         <v>-0.602121991185793</v>
       </c>
-      <c r="M4" t="n">
+      <c r="N4" t="n">
         <v>0.985250634561736</v>
       </c>
-      <c r="N4" t="n">
+      <c r="O4" t="n">
         <v>1.02429442096836</v>
       </c>
-      <c r="O4" t="n">
+      <c r="P4" t="n">
         <v>1.69756620097136</v>
       </c>
-      <c r="P4" t="n">
+      <c r="Q4" t="n">
         <v>2.05648417324653</v>
       </c>
-      <c r="Q4" t="n">
+      <c r="R4" t="n">
         <v>0.0156747398338641</v>
       </c>
-      <c r="R4" t="n">
+      <c r="S4" t="n">
         <v>0.479630186904212</v>
       </c>
-      <c r="S4" t="n">
+      <c r="T4" t="n">
         <v>1.55732102983817</v>
       </c>
-      <c r="T4" t="n">
+      <c r="U4" t="n">
         <v>-0.729997454146968</v>
       </c>
-      <c r="U4" t="n">
+      <c r="V4" t="n">
         <v>2.35392265133467</v>
       </c>
-      <c r="V4" t="n">
+      <c r="W4" t="n">
         <v>0.0379576527450984</v>
       </c>
-      <c r="W4" t="n">
+      <c r="X4" t="n">
         <v>-0.181719172844014</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" t="n">
         <v>0.135688031108185</v>
       </c>
-      <c r="B5" t="n">
+      <c r="C5" t="n">
         <v>1.49450464223431</v>
       </c>
-      <c r="C5" t="n">
+      <c r="D5" t="n">
         <v>0.0976357568493115</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>-0.188137301189861</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>0.282118725980557</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>0.0758358161710585</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>-0.225532053365704</v>
       </c>
-      <c r="H5" t="n">
+      <c r="I5" t="n">
         <v>-0.0769390706409609</v>
       </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
         <v>-0.545216549298544</v>
       </c>
-      <c r="J5" t="n">
+      <c r="K5" t="n">
         <v>0.414723455386916</v>
       </c>
-      <c r="K5" t="n">
+      <c r="L5" t="n">
         <v>-0.29335703816155</v>
       </c>
-      <c r="L5" t="n">
+      <c r="M5" t="n">
         <v>2.02487073476144</v>
       </c>
-      <c r="M5" t="n">
+      <c r="N5" t="n">
         <v>-0.0693496245178621</v>
       </c>
-      <c r="N5" t="n">
+      <c r="O5" t="n">
         <v>0.0000678103124660837</v>
       </c>
-      <c r="O5" t="n">
+      <c r="P5" t="n">
         <v>1.16883233408038</v>
       </c>
-      <c r="P5" t="n">
+      <c r="Q5" t="n">
         <v>-0.108451336028929</v>
       </c>
-      <c r="Q5" t="n">
+      <c r="R5" t="n">
         <v>-0.529800497361924</v>
       </c>
-      <c r="R5" t="n">
+      <c r="S5" t="n">
         <v>0.607317102240238</v>
       </c>
-      <c r="S5" t="n">
+      <c r="T5" t="n">
         <v>0.407230196830939</v>
       </c>
-      <c r="T5" t="n">
+      <c r="U5" t="n">
         <v>2.00304274776986</v>
       </c>
-      <c r="U5" t="n">
+      <c r="V5" t="n">
         <v>0.300209861197939</v>
       </c>
-      <c r="V5" t="n">
+      <c r="W5" t="n">
         <v>-0.944283417926256</v>
       </c>
-      <c r="W5" t="n">
+      <c r="X5" t="n">
         <v>0.57867935988357</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B6" t="n">
         <v>0.0770539733447342</v>
       </c>
-      <c r="B6" t="n">
+      <c r="C6" t="n">
         <v>0.302866400919668</v>
       </c>
-      <c r="C6" t="n">
+      <c r="D6" t="n">
         <v>-0.543608283194567</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>-0.622092390422354</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>-0.371674157594627</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>0.0935424165574429</v>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>-0.773833590414737</v>
       </c>
-      <c r="H6" t="n">
+      <c r="I6" t="n">
         <v>-0.238891873975283</v>
       </c>
-      <c r="I6" t="n">
+      <c r="J6" t="n">
         <v>-0.518356726906565</v>
       </c>
-      <c r="J6" t="n">
+      <c r="K6" t="n">
         <v>0.965469451024862</v>
       </c>
-      <c r="K6" t="n">
+      <c r="L6" t="n">
         <v>-0.450329848320705</v>
       </c>
-      <c r="L6" t="n">
+      <c r="M6" t="n">
         <v>-0.462336351651963</v>
       </c>
-      <c r="M6" t="n">
+      <c r="N6" t="n">
         <v>-0.451870169126869</v>
       </c>
-      <c r="N6" t="n">
+      <c r="O6" t="n">
         <v>-0.429895527145101</v>
       </c>
-      <c r="O6" t="n">
+      <c r="P6" t="n">
         <v>-0.115398217352912</v>
       </c>
-      <c r="P6" t="n">
+      <c r="Q6" t="n">
         <v>-1.17074776527235</v>
       </c>
-      <c r="Q6" t="n">
+      <c r="R6" t="n">
         <v>-0.0282186480166078</v>
       </c>
-      <c r="R6" t="n">
+      <c r="S6" t="n">
         <v>-0.450143119182933</v>
       </c>
-      <c r="S6" t="n">
+      <c r="T6" t="n">
         <v>-0.0668961705362156</v>
       </c>
-      <c r="T6" t="n">
+      <c r="U6" t="n">
         <v>-0.0841311171398445</v>
       </c>
-      <c r="U6" t="n">
+      <c r="V6" t="n">
         <v>-0.822599297549716</v>
       </c>
-      <c r="V6" t="n">
+      <c r="W6" t="n">
         <v>-0.0697523651244699</v>
       </c>
-      <c r="W6" t="n">
+      <c r="X6" t="n">
         <v>-0.106454589461453</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B7" t="n">
         <v>0.0404947882781174</v>
       </c>
-      <c r="B7" t="n">
+      <c r="C7" t="n">
         <v>-0.414864946813832</v>
       </c>
-      <c r="C7" t="n">
+      <c r="D7" t="n">
         <v>-0.550029577940684</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>-0.202125390528597</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>-0.19420037184982</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>0.360481945102388</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>0.198902735588543</v>
       </c>
-      <c r="H7" t="n">
+      <c r="I7" t="n">
         <v>-0.436059312312254</v>
       </c>
-      <c r="I7" t="n">
+      <c r="J7" t="n">
         <v>0.33187099832582</v>
       </c>
-      <c r="J7" t="n">
+      <c r="K7" t="n">
         <v>-0.0276786452588162</v>
       </c>
-      <c r="K7" t="n">
+      <c r="L7" t="n">
         <v>0.319813084885189</v>
       </c>
-      <c r="L7" t="n">
+      <c r="M7" t="n">
         <v>-0.621701855324189</v>
       </c>
-      <c r="M7" t="n">
+      <c r="N7" t="n">
         <v>-0.299058027469004</v>
       </c>
-      <c r="N7" t="n">
+      <c r="O7" t="n">
         <v>-0.27932529002674</v>
       </c>
-      <c r="O7" t="n">
+      <c r="P7" t="n">
         <v>-0.673578198506931</v>
       </c>
-      <c r="P7" t="n">
+      <c r="Q7" t="n">
         <v>0.0457403856232626</v>
       </c>
-      <c r="Q7" t="n">
+      <c r="R7" t="n">
         <v>0.690388115633142</v>
       </c>
-      <c r="R7" t="n">
+      <c r="S7" t="n">
         <v>-0.24327325241873</v>
       </c>
-      <c r="S7" t="n">
+      <c r="T7" t="n">
         <v>-0.688390957230675</v>
       </c>
-      <c r="T7" t="n">
+      <c r="U7" t="n">
         <v>-0.27353024844425</v>
       </c>
-      <c r="U7" t="n">
+      <c r="V7" t="n">
         <v>-0.715958845414613</v>
       </c>
-      <c r="V7" t="n">
+      <c r="W7" t="n">
         <v>1.20150507818257</v>
       </c>
-      <c r="W7" t="n">
+      <c r="X7" t="n">
         <v>-0.00474022315537953</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B8" t="n">
         <v>0.233917569677791</v>
       </c>
-      <c r="B8" t="n">
+      <c r="C8" t="n">
         <v>0.515471420320347</v>
       </c>
-      <c r="C8" t="n">
+      <c r="D8" t="n">
         <v>0.0175194910141728</v>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
         <v>-0.349484440304065</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>-0.386045205427395</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>-0.132722981608746</v>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>-0.490856712224145</v>
       </c>
-      <c r="H8" t="n">
+      <c r="I8" t="n">
         <v>-0.435661699754898</v>
       </c>
-      <c r="I8" t="n">
+      <c r="J8" t="n">
         <v>0.00187758403215112</v>
       </c>
-      <c r="J8" t="n">
+      <c r="K8" t="n">
         <v>-0.317804427028122</v>
       </c>
-      <c r="K8" t="n">
+      <c r="L8" t="n">
         <v>-0.281955876635323</v>
       </c>
-      <c r="L8" t="n">
+      <c r="M8" t="n">
         <v>0.317354110589388</v>
       </c>
-      <c r="M8" t="n">
+      <c r="N8" t="n">
         <v>-0.307610360655606</v>
       </c>
-      <c r="N8" t="n">
+      <c r="O8" t="n">
         <v>-0.256221081712159</v>
       </c>
-      <c r="O8" t="n">
+      <c r="P8" t="n">
         <v>-0.637193249610474</v>
       </c>
-      <c r="P8" t="n">
+      <c r="Q8" t="n">
         <v>-0.250322246252809</v>
       </c>
-      <c r="Q8" t="n">
+      <c r="R8" t="n">
         <v>-0.0283271227076605</v>
       </c>
-      <c r="R8" t="n">
+      <c r="S8" t="n">
         <v>0.186103595560284</v>
       </c>
-      <c r="S8" t="n">
+      <c r="T8" t="n">
         <v>-0.247836497742732</v>
       </c>
-      <c r="T8" t="n">
+      <c r="U8" t="n">
         <v>0.349563457904469</v>
       </c>
-      <c r="U8" t="n">
+      <c r="V8" t="n">
         <v>-0.421963532837897</v>
       </c>
-      <c r="V8" t="n">
+      <c r="W8" t="n">
         <v>-0.333318532719887</v>
       </c>
-      <c r="W8" t="n">
+      <c r="X8" t="n">
         <v>0.0455477488219248</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
+      <c r="A9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B9" t="n">
         <v>-0.465745865029967</v>
       </c>
-      <c r="B9" t="n">
+      <c r="C9" t="n">
         <v>-0.2499908690813</v>
       </c>
-      <c r="C9" t="n">
+      <c r="D9" t="n">
         <v>-0.523146901586802</v>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
         <v>-0.382605772579067</v>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>-0.401096887363094</v>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
         <v>1.23067669727648</v>
       </c>
-      <c r="G9" t="n">
+      <c r="H9" t="n">
         <v>-0.326588292719027</v>
       </c>
-      <c r="H9" t="n">
+      <c r="I9" t="n">
         <v>-0.476866432720395</v>
       </c>
-      <c r="I9" t="n">
+      <c r="J9" t="n">
         <v>-0.746585733035012</v>
       </c>
-      <c r="J9" t="n">
+      <c r="K9" t="n">
         <v>-0.604990942230045</v>
       </c>
-      <c r="K9" t="n">
+      <c r="L9" t="n">
         <v>-0.555347965591385</v>
       </c>
-      <c r="L9" t="n">
+      <c r="M9" t="n">
         <v>0.28206957720551</v>
       </c>
-      <c r="M9" t="n">
+      <c r="N9" t="n">
         <v>-0.495274136583367</v>
       </c>
-      <c r="N9" t="n">
+      <c r="O9" t="n">
         <v>-0.175167885440641</v>
       </c>
-      <c r="O9" t="n">
+      <c r="P9" t="n">
         <v>-0.375201162214969</v>
       </c>
-      <c r="P9" t="n">
+      <c r="Q9" t="n">
         <v>-0.27532536379984</v>
       </c>
-      <c r="Q9" t="n">
+      <c r="R9" t="n">
         <v>-0.108285720636435</v>
       </c>
-      <c r="R9" t="n">
+      <c r="S9" t="n">
         <v>-0.755554641409861</v>
       </c>
-      <c r="S9" t="n">
+      <c r="T9" t="n">
         <v>-0.533973774913479</v>
       </c>
-      <c r="T9" t="n">
+      <c r="U9" t="n">
         <v>-0.130053758599217</v>
       </c>
-      <c r="U9" t="n">
+      <c r="V9" t="n">
         <v>-0.470142474233395</v>
       </c>
-      <c r="V9" t="n">
+      <c r="W9" t="n">
         <v>-0.59760434877578</v>
       </c>
-      <c r="W9" t="n">
+      <c r="X9" t="n">
         <v>-0.62420995411974</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
+      <c r="A10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B10" t="n">
         <v>0.345911669571026</v>
       </c>
-      <c r="B10" t="n">
+      <c r="C10" t="n">
         <v>-1.03329301267967</v>
       </c>
-      <c r="C10" t="n">
+      <c r="D10" t="n">
         <v>-0.405759961565337</v>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
         <v>-0.186141639941228</v>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
         <v>-0.396506514524694</v>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
         <v>-0.68773868429233</v>
       </c>
-      <c r="G10" t="n">
+      <c r="H10" t="n">
         <v>0.256595210123654</v>
       </c>
-      <c r="H10" t="n">
+      <c r="I10" t="n">
         <v>-0.377445873253773</v>
       </c>
-      <c r="I10" t="n">
+      <c r="J10" t="n">
         <v>-0.19230305466677</v>
       </c>
-      <c r="J10" t="n">
+      <c r="K10" t="n">
         <v>-0.388814598292494</v>
       </c>
-      <c r="K10" t="n">
+      <c r="L10" t="n">
         <v>-0.243835876051517</v>
       </c>
-      <c r="L10" t="n">
+      <c r="M10" t="n">
         <v>-1.00446557509809</v>
       </c>
-      <c r="M10" t="n">
+      <c r="N10" t="n">
         <v>0.111306023171069</v>
       </c>
-      <c r="N10" t="n">
+      <c r="O10" t="n">
         <v>-0.250222112844393</v>
       </c>
-      <c r="O10" t="n">
+      <c r="P10" t="n">
         <v>-0.138704437002629</v>
       </c>
-      <c r="P10" t="n">
+      <c r="Q10" t="n">
         <v>0.216915663236609</v>
       </c>
-      <c r="Q10" t="n">
+      <c r="R10" t="n">
         <v>0.0784187222832774</v>
       </c>
-      <c r="R10" t="n">
+      <c r="S10" t="n">
         <v>-0.439531273745602</v>
       </c>
-      <c r="S10" t="n">
+      <c r="T10" t="n">
         <v>-0.535454755478304</v>
       </c>
-      <c r="T10" t="n">
+      <c r="U10" t="n">
         <v>-0.787326011992009</v>
       </c>
-      <c r="U10" t="n">
+      <c r="V10" t="n">
         <v>-0.463467599919065</v>
       </c>
-      <c r="V10" t="n">
+      <c r="W10" t="n">
         <v>0.30183090866006</v>
       </c>
-      <c r="W10" t="n">
+      <c r="X10" t="n">
         <v>-0.30435700935969</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="n">
         <v>-0.593846267368161</v>
       </c>
-      <c r="B11" t="n">
+      <c r="C11" t="n">
         <v>-1.15414279081911</v>
       </c>
-      <c r="C11" t="n">
+      <c r="D11" t="n">
         <v>0.998990577241354</v>
       </c>
-      <c r="D11" t="n">
+      <c r="E11" t="n">
         <v>1.05681282892511</v>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
         <v>0.596669068673392</v>
       </c>
-      <c r="F11" t="n">
+      <c r="G11" t="n">
         <v>-0.595390525450417</v>
       </c>
-      <c r="G11" t="n">
+      <c r="H11" t="n">
         <v>0.7703244841088</v>
       </c>
-      <c r="H11" t="n">
+      <c r="I11" t="n">
         <v>1.20676729504782</v>
       </c>
-      <c r="I11" t="n">
+      <c r="J11" t="n">
         <v>1.34117651426268</v>
       </c>
-      <c r="J11" t="n">
+      <c r="K11" t="n">
         <v>-0.0881588100492298</v>
       </c>
-      <c r="K11" t="n">
+      <c r="L11" t="n">
         <v>0.960811764156139</v>
       </c>
-      <c r="L11" t="n">
+      <c r="M11" t="n">
         <v>-1.20180605404257</v>
       </c>
-      <c r="M11" t="n">
+      <c r="N11" t="n">
         <v>0.930750035417141</v>
       </c>
-      <c r="N11" t="n">
+      <c r="O11" t="n">
         <v>0.869075419603146</v>
       </c>
-      <c r="O11" t="n">
+      <c r="P11" t="n">
         <v>0.0794820990614283</v>
       </c>
-      <c r="P11" t="n">
+      <c r="Q11" t="n">
         <v>0.60793121771483</v>
       </c>
-      <c r="Q11" t="n">
+      <c r="R11" t="n">
         <v>0.294458311327927</v>
       </c>
-      <c r="R11" t="n">
+      <c r="S11" t="n">
         <v>0.39402647714176</v>
       </c>
-      <c r="S11" t="n">
+      <c r="T11" t="n">
         <v>0.723846022331551</v>
       </c>
-      <c r="T11" t="n">
+      <c r="U11" t="n">
         <v>-1.27193493907841</v>
       </c>
-      <c r="U11" t="n">
+      <c r="V11" t="n">
         <v>1.03180538097325</v>
       </c>
-      <c r="V11" t="n">
+      <c r="W11" t="n">
         <v>0.933270914272267</v>
       </c>
-      <c r="W11" t="n">
+      <c r="X11" t="n">
         <v>0.0808862506754261</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
+      <c r="A12" t="s">
+        <v>126</v>
+      </c>
+      <c r="B12" t="n">
         <v>-0.753265289843352</v>
       </c>
-      <c r="B12" t="n">
+      <c r="C12" t="n">
         <v>-0.791588888631569</v>
       </c>
-      <c r="C12" t="n">
+      <c r="D12" t="n">
         <v>0.957609756671358</v>
       </c>
-      <c r="D12" t="n">
+      <c r="E12" t="n">
         <v>0.437698364532612</v>
       </c>
-      <c r="E12" t="n">
+      <c r="F12" t="n">
         <v>0.862998241715303</v>
       </c>
-      <c r="F12" t="n">
+      <c r="G12" t="n">
         <v>-0.661442096531054</v>
       </c>
-      <c r="G12" t="n">
+      <c r="H12" t="n">
         <v>-0.773223588730698</v>
       </c>
-      <c r="H12" t="n">
+      <c r="I12" t="n">
         <v>1.41822816983595</v>
       </c>
-      <c r="I12" t="n">
+      <c r="J12" t="n">
         <v>0.742946347015174</v>
       </c>
-      <c r="J12" t="n">
+      <c r="K12" t="n">
         <v>-0.752222956623928</v>
       </c>
-      <c r="K12" t="n">
+      <c r="L12" t="n">
         <v>0.1323415504395</v>
       </c>
-      <c r="L12" t="n">
+      <c r="M12" t="n">
         <v>-0.803215969096286</v>
       </c>
-      <c r="M12" t="n">
+      <c r="N12" t="n">
         <v>-0.493833001348481</v>
       </c>
-      <c r="N12" t="n">
+      <c r="O12" t="n">
         <v>0.404717660976818</v>
       </c>
-      <c r="O12" t="n">
+      <c r="P12" t="n">
         <v>-0.77193424762943</v>
       </c>
-      <c r="P12" t="n">
+      <c r="Q12" t="n">
         <v>2.09650931336335</v>
       </c>
-      <c r="Q12" t="n">
+      <c r="R12" t="n">
         <v>-0.533018976310836</v>
       </c>
-      <c r="R12" t="n">
+      <c r="S12" t="n">
         <v>0.943285805333189</v>
       </c>
-      <c r="S12" t="n">
+      <c r="T12" t="n">
         <v>0.88340851603469</v>
       </c>
-      <c r="T12" t="n">
+      <c r="U12" t="n">
         <v>-0.738082653477906</v>
       </c>
-      <c r="U12" t="n">
+      <c r="V12" t="n">
         <v>-0.414336128779038</v>
       </c>
-      <c r="V12" t="n">
+      <c r="W12" t="n">
         <v>-0.794647627797327</v>
       </c>
-      <c r="W12" t="n">
+      <c r="X12" t="n">
         <v>-0.79563292185626</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
+      <c r="A13" t="s">
+        <v>127</v>
+      </c>
+      <c r="B13" t="n">
         <v>-0.575551396360498</v>
       </c>
-      <c r="B13" t="n">
+      <c r="C13" t="n">
         <v>-0.646793349048476</v>
       </c>
-      <c r="C13" t="n">
+      <c r="D13" t="n">
         <v>0.507786831736535</v>
       </c>
-      <c r="D13" t="n">
+      <c r="E13" t="n">
         <v>2.33472417593212</v>
       </c>
-      <c r="E13" t="n">
+      <c r="F13" t="n">
         <v>1.29272186315313</v>
       </c>
-      <c r="F13" t="n">
+      <c r="G13" t="n">
         <v>0.127351894897867</v>
       </c>
-      <c r="G13" t="n">
+      <c r="H13" t="n">
         <v>-0.901145965905741</v>
       </c>
-      <c r="H13" t="n">
+      <c r="I13" t="n">
         <v>0.467603824671809</v>
       </c>
-      <c r="I13" t="n">
+      <c r="J13" t="n">
         <v>0.657900790574586</v>
       </c>
-      <c r="J13" t="n">
+      <c r="K13" t="n">
         <v>0.0032767656540103</v>
       </c>
-      <c r="K13" t="n">
+      <c r="L13" t="n">
         <v>1.95368717217853</v>
       </c>
-      <c r="L13" t="n">
+      <c r="M13" t="n">
         <v>-0.842924480205492</v>
       </c>
-      <c r="M13" t="n">
+      <c r="N13" t="n">
         <v>0.808126234735768</v>
       </c>
-      <c r="N13" t="n">
+      <c r="O13" t="n">
         <v>0.863119369272829</v>
       </c>
-      <c r="O13" t="n">
+      <c r="P13" t="n">
         <v>-0.879820735538346</v>
       </c>
-      <c r="P13" t="n">
+      <c r="Q13" t="n">
         <v>-0.414851011182359</v>
       </c>
-      <c r="Q13" t="n">
+      <c r="R13" t="n">
         <v>-0.70191546898585</v>
       </c>
-      <c r="R13" t="n">
+      <c r="S13" t="n">
         <v>1.00259321231163</v>
       </c>
-      <c r="S13" t="n">
+      <c r="T13" t="n">
         <v>-0.24356047140334</v>
       </c>
-      <c r="T13" t="n">
+      <c r="U13" t="n">
         <v>-0.801242547918978</v>
       </c>
-      <c r="U13" t="n">
+      <c r="V13" t="n">
         <v>-0.544968738505398</v>
       </c>
-      <c r="V13" t="n">
+      <c r="W13" t="n">
         <v>-0.985476965398001</v>
       </c>
-      <c r="W13" t="n">
+      <c r="X13" t="n">
         <v>-0.919687357008204</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
+      <c r="A14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B14" t="n">
         <v>-0.205734423789736</v>
       </c>
-      <c r="B14" t="n">
+      <c r="C14" t="n">
         <v>0.870982793371001</v>
       </c>
-      <c r="C14" t="n">
+      <c r="D14" t="n">
         <v>0.129596335797766</v>
       </c>
-      <c r="D14" t="n">
+      <c r="E14" t="n">
         <v>-0.530890946522053</v>
       </c>
-      <c r="E14" t="n">
+      <c r="F14" t="n">
         <v>-0.0219976578598537</v>
       </c>
-      <c r="F14" t="n">
+      <c r="G14" t="n">
         <v>1.55217489105105</v>
       </c>
-      <c r="G14" t="n">
+      <c r="H14" t="n">
         <v>-0.725760807071407</v>
       </c>
-      <c r="H14" t="n">
+      <c r="I14" t="n">
         <v>-0.51746363497366</v>
       </c>
-      <c r="I14" t="n">
+      <c r="J14" t="n">
         <v>-0.0176958391691852</v>
       </c>
-      <c r="J14" t="n">
+      <c r="K14" t="n">
         <v>1.13280383417234</v>
       </c>
-      <c r="K14" t="n">
+      <c r="L14" t="n">
         <v>0.0190378386876468</v>
       </c>
-      <c r="L14" t="n">
+      <c r="M14" t="n">
         <v>-0.580966179555527</v>
       </c>
-      <c r="M14" t="n">
+      <c r="N14" t="n">
         <v>0.622234040738586</v>
       </c>
-      <c r="N14" t="n">
+      <c r="O14" t="n">
         <v>0.0890140401562253</v>
       </c>
-      <c r="O14" t="n">
+      <c r="P14" t="n">
         <v>-0.0285723393823273</v>
       </c>
-      <c r="P14" t="n">
+      <c r="Q14" t="n">
         <v>-0.393713187402756</v>
       </c>
-      <c r="Q14" t="n">
+      <c r="R14" t="n">
         <v>-0.723169081514</v>
       </c>
-      <c r="R14" t="n">
+      <c r="S14" t="n">
         <v>-0.531537970216421</v>
       </c>
-      <c r="S14" t="n">
+      <c r="T14" t="n">
         <v>-0.638880838757158</v>
       </c>
-      <c r="T14" t="n">
+      <c r="U14" t="n">
         <v>-0.576387857934643</v>
       </c>
-      <c r="U14" t="n">
+      <c r="V14" t="n">
         <v>-0.534815747614707</v>
       </c>
-      <c r="V14" t="n">
+      <c r="W14" t="n">
         <v>-0.870031073821448</v>
       </c>
-      <c r="W14" t="n">
+      <c r="X14" t="n">
         <v>-0.0696761634730108</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
+      <c r="A15" t="s">
+        <v>129</v>
+      </c>
+      <c r="B15" t="n">
         <v>-0.0444900805219199</v>
       </c>
-      <c r="B15" t="n">
+      <c r="C15" t="n">
         <v>-0.626580324170176</v>
       </c>
-      <c r="C15" t="n">
+      <c r="D15" t="n">
         <v>0.139015530391162</v>
       </c>
-      <c r="D15" t="n">
+      <c r="E15" t="n">
         <v>0.122368608608379</v>
       </c>
-      <c r="E15" t="n">
+      <c r="F15" t="n">
         <v>-0.532005296955358</v>
       </c>
-      <c r="F15" t="n">
+      <c r="G15" t="n">
         <v>0.382125072651379</v>
       </c>
-      <c r="G15" t="n">
+      <c r="H15" t="n">
         <v>1.20335025107636</v>
       </c>
-      <c r="H15" t="n">
+      <c r="I15" t="n">
         <v>0.324186851998935</v>
       </c>
-      <c r="I15" t="n">
+      <c r="J15" t="n">
         <v>-0.2679349630077</v>
       </c>
-      <c r="J15" t="n">
+      <c r="K15" t="n">
         <v>-0.742637008541527</v>
       </c>
-      <c r="K15" t="n">
+      <c r="L15" t="n">
         <v>0.227313993572846</v>
       </c>
-      <c r="L15" t="n">
+      <c r="M15" t="n">
         <v>-0.692009713828217</v>
       </c>
-      <c r="M15" t="n">
+      <c r="N15" t="n">
         <v>1.63616277162404</v>
       </c>
-      <c r="N15" t="n">
+      <c r="O15" t="n">
         <v>-0.521461362343701</v>
       </c>
-      <c r="O15" t="n">
+      <c r="P15" t="n">
         <v>0.366329765453922</v>
       </c>
-      <c r="P15" t="n">
+      <c r="Q15" t="n">
         <v>-0.387954369046413</v>
       </c>
-      <c r="Q15" t="n">
+      <c r="R15" t="n">
         <v>2.33497232079654</v>
       </c>
-      <c r="R15" t="n">
+      <c r="S15" t="n">
         <v>-0.497012108866951</v>
       </c>
-      <c r="S15" t="n">
+      <c r="T15" t="n">
         <v>0.773098013141497</v>
       </c>
-      <c r="T15" t="n">
+      <c r="U15" t="n">
         <v>-0.705764799494448</v>
       </c>
-      <c r="U15" t="n">
+      <c r="V15" t="n">
         <v>1.63785660294322</v>
       </c>
-      <c r="V15" t="n">
+      <c r="W15" t="n">
         <v>2.43522573435228</v>
       </c>
-      <c r="W15" t="n">
+      <c r="X15" t="n">
         <v>-0.690535415278506</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="n">
+      <c r="A16" t="s">
+        <v>130</v>
+      </c>
+      <c r="B16" t="n">
         <v>0.0894019623800398</v>
       </c>
-      <c r="B16" t="n">
+      <c r="C16" t="n">
         <v>0.90187406248223</v>
       </c>
-      <c r="C16" t="n">
+      <c r="D16" t="n">
         <v>-0.802758891834407</v>
       </c>
-      <c r="D16" t="n">
+      <c r="E16" t="n">
         <v>-0.675112897339848</v>
       </c>
-      <c r="E16" t="n">
+      <c r="F16" t="n">
         <v>-0.681297072238712</v>
       </c>
-      <c r="F16" t="n">
+      <c r="G16" t="n">
         <v>1.20696410799265</v>
       </c>
-      <c r="G16" t="n">
+      <c r="H16" t="n">
         <v>2.25160615149497</v>
       </c>
-      <c r="H16" t="n">
+      <c r="I16" t="n">
         <v>-0.529309040136736</v>
       </c>
-      <c r="I16" t="n">
+      <c r="J16" t="n">
         <v>-0.475144747089425</v>
       </c>
-      <c r="J16" t="n">
+      <c r="K16" t="n">
         <v>0.707131298751438</v>
       </c>
-      <c r="K16" t="n">
+      <c r="L16" t="n">
         <v>-0.204839696657985</v>
       </c>
-      <c r="L16" t="n">
+      <c r="M16" t="n">
         <v>0.38030389757025</v>
       </c>
-      <c r="M16" t="n">
+      <c r="N16" t="n">
         <v>-0.615962016210663</v>
       </c>
-      <c r="N16" t="n">
+      <c r="O16" t="n">
         <v>-0.420657321900764</v>
       </c>
-      <c r="O16" t="n">
+      <c r="P16" t="n">
         <v>2.47712190322863</v>
       </c>
-      <c r="P16" t="n">
+      <c r="Q16" t="n">
         <v>-0.765851701117687</v>
       </c>
-      <c r="Q16" t="n">
+      <c r="R16" t="n">
         <v>-0.178098541186874</v>
       </c>
-      <c r="R16" t="n">
+      <c r="S16" t="n">
         <v>-0.493097087701602</v>
       </c>
-      <c r="S16" t="n">
+      <c r="T16" t="n">
         <v>-0.63904602406547</v>
       </c>
-      <c r="T16" t="n">
+      <c r="U16" t="n">
         <v>0.475266302219576</v>
       </c>
-      <c r="U16" t="n">
+      <c r="V16" t="n">
         <v>-0.379219344898934</v>
       </c>
-      <c r="V16" t="n">
+      <c r="W16" t="n">
         <v>-0.580045479112795</v>
       </c>
-      <c r="W16" t="n">
+      <c r="X16" t="n">
         <v>-0.475564655229996</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="n">
+      <c r="A17" t="s">
+        <v>131</v>
+      </c>
+      <c r="B17" t="n">
         <v>-0.129137395127345</v>
       </c>
-      <c r="B17" t="n">
+      <c r="C17" t="n">
         <v>-0.245281255939389</v>
       </c>
-      <c r="C17" t="n">
+      <c r="D17" t="n">
         <v>-0.319456439820845</v>
       </c>
-      <c r="D17" t="n">
+      <c r="E17" t="n">
         <v>-0.321374071106152</v>
       </c>
-      <c r="E17" t="n">
+      <c r="F17" t="n">
         <v>-0.313951080534249</v>
       </c>
-      <c r="F17" t="n">
+      <c r="G17" t="n">
         <v>-0.178326355390406</v>
       </c>
-      <c r="G17" t="n">
+      <c r="H17" t="n">
         <v>0.0741798703001086</v>
       </c>
-      <c r="H17" t="n">
+      <c r="I17" t="n">
         <v>-0.307928359181948</v>
       </c>
-      <c r="I17" t="n">
+      <c r="J17" t="n">
         <v>-0.290496297771228</v>
       </c>
-      <c r="J17" t="n">
+      <c r="K17" t="n">
         <v>0.326334467880177</v>
       </c>
-      <c r="K17" t="n">
+      <c r="L17" t="n">
         <v>-0.308265489025616</v>
       </c>
-      <c r="L17" t="n">
+      <c r="M17" t="n">
         <v>-0.00586129715888197</v>
       </c>
-      <c r="M17" t="n">
+      <c r="N17" t="n">
         <v>-0.316718843605564</v>
       </c>
-      <c r="N17" t="n">
+      <c r="O17" t="n">
         <v>-0.161733019968742</v>
       </c>
-      <c r="O17" t="n">
+      <c r="P17" t="n">
         <v>-0.251744028003077</v>
       </c>
-      <c r="P17" t="n">
+      <c r="Q17" t="n">
         <v>-0.303160793498876</v>
       </c>
-      <c r="Q17" t="n">
+      <c r="R17" t="n">
         <v>-0.284113117857983</v>
       </c>
-      <c r="R17" t="n">
+      <c r="S17" t="n">
         <v>-0.289932757371378</v>
       </c>
-      <c r="S17" t="n">
+      <c r="T17" t="n">
         <v>-0.318383885769756</v>
       </c>
-      <c r="T17" t="n">
+      <c r="U17" t="n">
         <v>0.393425795089351</v>
       </c>
-      <c r="U17" t="n">
+      <c r="V17" t="n">
         <v>0.122509630753378</v>
       </c>
-      <c r="V17" t="n">
+      <c r="W17" t="n">
         <v>1.34410325053068</v>
       </c>
-      <c r="W17" t="n">
+      <c r="X17" t="n">
         <v>0.976908679655748</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="n">
+      <c r="A18" t="s">
+        <v>132</v>
+      </c>
+      <c r="B18" t="n">
         <v>-0.461719464901485</v>
       </c>
-      <c r="B18" t="n">
+      <c r="C18" t="n">
         <v>-0.443212011398654</v>
       </c>
-      <c r="C18" t="n">
+      <c r="D18" t="n">
         <v>-0.52577700593981</v>
       </c>
-      <c r="D18" t="n">
+      <c r="E18" t="n">
         <v>-0.525908312086709</v>
       </c>
-      <c r="E18" t="n">
+      <c r="F18" t="n">
         <v>-0.517035463720882</v>
       </c>
-      <c r="F18" t="n">
+      <c r="G18" t="n">
         <v>-0.507989334221928</v>
       </c>
-      <c r="G18" t="n">
+      <c r="H18" t="n">
         <v>-0.0439912075210081</v>
       </c>
-      <c r="H18" t="n">
+      <c r="I18" t="n">
         <v>-0.468732627432272</v>
       </c>
-      <c r="I18" t="n">
+      <c r="J18" t="n">
         <v>-0.121222359679859</v>
       </c>
-      <c r="J18" t="n">
+      <c r="K18" t="n">
         <v>0.242200241791388</v>
       </c>
-      <c r="K18" t="n">
+      <c r="L18" t="n">
         <v>-0.373734634308963</v>
       </c>
-      <c r="L18" t="n">
+      <c r="M18" t="n">
         <v>1.95368516456214</v>
       </c>
-      <c r="M18" t="n">
+      <c r="N18" t="n">
         <v>-0.524517711539196</v>
       </c>
-      <c r="N18" t="n">
+      <c r="O18" t="n">
         <v>-0.288497469895774</v>
       </c>
-      <c r="O18" t="n">
+      <c r="P18" t="n">
         <v>0.0159393682196303</v>
       </c>
-      <c r="P18" t="n">
+      <c r="Q18" t="n">
         <v>-0.282159704667895</v>
       </c>
-      <c r="Q18" t="n">
+      <c r="R18" t="n">
         <v>-0.502107806612864</v>
       </c>
-      <c r="R18" t="n">
+      <c r="S18" t="n">
         <v>-0.514343867902819</v>
       </c>
-      <c r="S18" t="n">
+      <c r="T18" t="n">
         <v>-0.52217738356536</v>
       </c>
-      <c r="T18" t="n">
+      <c r="U18" t="n">
         <v>1.82059587713102</v>
       </c>
-      <c r="U18" t="n">
+      <c r="V18" t="n">
         <v>-0.491676587343349</v>
       </c>
-      <c r="V18" t="n">
+      <c r="W18" t="n">
         <v>-0.458178581560971</v>
       </c>
-      <c r="W18" t="n">
+      <c r="X18" t="n">
         <v>1.16119672402963</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="n">
+      <c r="A19" t="s">
+        <v>133</v>
+      </c>
+      <c r="B19" t="n">
         <v>1.19267706091775</v>
       </c>
-      <c r="B19" t="n">
+      <c r="C19" t="n">
         <v>-0.301052525341922</v>
       </c>
-      <c r="C19" t="n">
+      <c r="D19" t="n">
         <v>0.400086440006511</v>
       </c>
-      <c r="D19" t="n">
+      <c r="E19" t="n">
         <v>0.752966900840336</v>
       </c>
-      <c r="E19" t="n">
+      <c r="F19" t="n">
         <v>0.739135356142898</v>
       </c>
-      <c r="F19" t="n">
+      <c r="G19" t="n">
         <v>-1.07487700452682</v>
       </c>
-      <c r="G19" t="n">
+      <c r="H19" t="n">
         <v>0.0975570138874772</v>
       </c>
-      <c r="H19" t="n">
+      <c r="I19" t="n">
         <v>-0.0940086036329307</v>
       </c>
-      <c r="I19" t="n">
+      <c r="J19" t="n">
         <v>-0.295805526537364</v>
       </c>
-      <c r="J19" t="n">
+      <c r="K19" t="n">
         <v>-0.170151998725486</v>
       </c>
-      <c r="K19" t="n">
+      <c r="L19" t="n">
         <v>-0.298365811858222</v>
       </c>
-      <c r="L19" t="n">
+      <c r="M19" t="n">
         <v>0.0659726205263397</v>
       </c>
-      <c r="M19" t="n">
+      <c r="N19" t="n">
         <v>-0.680706980884602</v>
       </c>
-      <c r="N19" t="n">
+      <c r="O19" t="n">
         <v>0.731435671047399</v>
       </c>
-      <c r="O19" t="n">
+      <c r="P19" t="n">
         <v>-0.629644603624357</v>
       </c>
-      <c r="P19" t="n">
+      <c r="Q19" t="n">
         <v>0.504763410749726</v>
       </c>
-      <c r="Q19" t="n">
+      <c r="R19" t="n">
         <v>1.19942050992602</v>
       </c>
-      <c r="R19" t="n">
+      <c r="S19" t="n">
         <v>0.764445140722727</v>
       </c>
-      <c r="S19" t="n">
+      <c r="T19" t="n">
         <v>1.08579046865762</v>
       </c>
-      <c r="T19" t="n">
+      <c r="U19" t="n">
         <v>-0.364875457478697</v>
       </c>
-      <c r="U19" t="n">
+      <c r="V19" t="n">
         <v>0.529816936057543</v>
       </c>
-      <c r="V19" t="n">
+      <c r="W19" t="n">
         <v>-0.138481719341181</v>
       </c>
-      <c r="W19" t="n">
+      <c r="X19" t="n">
         <v>-0.10087137914155</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="n">
+      <c r="A20" t="s">
+        <v>134</v>
+      </c>
+      <c r="B20" t="n">
         <v>1.55915149151557</v>
       </c>
-      <c r="B20" t="n">
+      <c r="C20" t="n">
         <v>1.51178286295268</v>
       </c>
-      <c r="C20" t="n">
+      <c r="D20" t="n">
         <v>-0.766462374315664</v>
       </c>
-      <c r="D20" t="n">
+      <c r="E20" t="n">
         <v>-1.12500739453955</v>
       </c>
-      <c r="E20" t="n">
+      <c r="F20" t="n">
         <v>-0.686614833628492</v>
       </c>
-      <c r="F20" t="n">
+      <c r="G20" t="n">
         <v>-0.793447341538777</v>
       </c>
-      <c r="G20" t="n">
+      <c r="H20" t="n">
         <v>-0.503472638082524</v>
       </c>
-      <c r="H20" t="n">
+      <c r="I20" t="n">
         <v>-0.901988217179735</v>
       </c>
-      <c r="I20" t="n">
+      <c r="J20" t="n">
         <v>-0.316814936448309</v>
       </c>
-      <c r="J20" t="n">
+      <c r="K20" t="n">
         <v>-0.294968486980585</v>
       </c>
-      <c r="K20" t="n">
+      <c r="L20" t="n">
         <v>-1.01522515708039</v>
       </c>
-      <c r="L20" t="n">
+      <c r="M20" t="n">
         <v>0.840194781016257</v>
       </c>
-      <c r="M20" t="n">
+      <c r="N20" t="n">
         <v>-0.709857796440463</v>
       </c>
-      <c r="N20" t="n">
+      <c r="O20" t="n">
         <v>-0.408428270177506</v>
       </c>
-      <c r="O20" t="n">
+      <c r="P20" t="n">
         <v>0.132602633438499</v>
       </c>
-      <c r="P20" t="n">
+      <c r="Q20" t="n">
         <v>-0.806939461985724</v>
       </c>
-      <c r="Q20" t="n">
+      <c r="R20" t="n">
         <v>-0.234940129843345</v>
       </c>
-      <c r="R20" t="n">
+      <c r="S20" t="n">
         <v>-0.275689548793253</v>
       </c>
-      <c r="S20" t="n">
+      <c r="T20" t="n">
         <v>-0.469835173122079</v>
       </c>
-      <c r="T20" t="n">
+      <c r="U20" t="n">
         <v>0.646800454142474</v>
       </c>
-      <c r="U20" t="n">
+      <c r="V20" t="n">
         <v>0.13496023829927</v>
       </c>
-      <c r="V20" t="n">
+      <c r="W20" t="n">
         <v>-0.194702699889872</v>
       </c>
-      <c r="W20" t="n">
+      <c r="X20" t="n">
         <v>0.931326995681454</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Figure 3A notebook, scripts and output
</commit_message>
<xml_diff>
--- a/tables/mutational_signatures.xlsx
+++ b/tables/mutational_signatures.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
   <si>
     <t xml:space="preserve">patient_id</t>
   </si>
@@ -294,9 +294,6 @@
     <t xml:space="preserve">SPECTRUM-OV-123</t>
   </si>
   <si>
-    <t xml:space="preserve">topic</t>
-  </si>
-  <si>
     <t xml:space="preserve">063</t>
   </si>
   <si>
@@ -364,60 +361,6 @@
   </si>
   <si>
     <t xml:space="preserve">083</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Age</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SBS5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SBS8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SBS40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">POLH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MMRD1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MMRD2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APOBEC1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APOBEC2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S-Dup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M-Dup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L-Dup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S-Del</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L-Del</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clust-FBI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clust-SV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FBI/Inv</t>
   </si>
 </sst>
 </file>
@@ -1851,1413 +1794,1353 @@
       <c r="W1" t="s">
         <v>115</v>
       </c>
-      <c r="X1" t="s">
-        <v>116</v>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>117</v>
+      <c r="A2" t="n">
+        <v>0.55867102797821</v>
       </c>
       <c r="B2" t="n">
-        <v>0.55867102797821</v>
+        <v>0.653823517920692</v>
       </c>
       <c r="C2" t="n">
-        <v>0.653823517920692</v>
+        <v>-0.337416099799313</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.337416099799313</v>
+        <v>-0.379195664522017</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.379195664522017</v>
+        <v>-0.388345311851232</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.388345311851232</v>
+        <v>-0.370290032650612</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.370290032650612</v>
+        <v>-0.405740686540713</v>
       </c>
       <c r="H2" t="n">
-        <v>-0.405740686540713</v>
+        <v>-0.416759970706528</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.416759970706528</v>
+        <v>-0.314890984850368</v>
       </c>
       <c r="J2" t="n">
-        <v>-0.314890984850368</v>
+        <v>-0.175396651095867</v>
       </c>
       <c r="K2" t="n">
-        <v>-0.175396651095867</v>
+        <v>-0.379036366438699</v>
       </c>
       <c r="L2" t="n">
-        <v>-0.379036366438699</v>
+        <v>0.614015866517648</v>
       </c>
       <c r="M2" t="n">
-        <v>0.614015866517648</v>
+        <v>-0.375890809350173</v>
       </c>
       <c r="N2" t="n">
-        <v>-0.375890809350173</v>
+        <v>-0.367534703000738</v>
       </c>
       <c r="O2" t="n">
-        <v>-0.367534703000738</v>
+        <v>-0.414438563432522</v>
       </c>
       <c r="P2" t="n">
-        <v>-0.414438563432522</v>
+        <v>-0.406328020619258</v>
       </c>
       <c r="Q2" t="n">
-        <v>-0.406328020619258</v>
+        <v>-0.329107086311861</v>
       </c>
       <c r="R2" t="n">
-        <v>-0.329107086311861</v>
+        <v>-0.131914228789296</v>
       </c>
       <c r="S2" t="n">
-        <v>-0.131914228789296</v>
+        <v>-0.402455942894852</v>
       </c>
       <c r="T2" t="n">
-        <v>-0.402455942894852</v>
+        <v>0.968983406002764</v>
       </c>
       <c r="U2" t="n">
-        <v>0.968983406002764</v>
+        <v>-0.420263278255262</v>
       </c>
       <c r="V2" t="n">
-        <v>-0.420263278255262</v>
+        <v>-0.372989391074907</v>
       </c>
       <c r="W2" t="n">
-        <v>-0.372989391074907</v>
-      </c>
-      <c r="X2" t="n">
         <v>0.00259478318362204</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
-        <v>118</v>
+      <c r="A3" t="n">
+        <v>1.46191212775567</v>
       </c>
       <c r="B3" t="n">
-        <v>1.46191212775567</v>
+        <v>1.6547219708436</v>
       </c>
       <c r="C3" t="n">
-        <v>1.6547219708436</v>
+        <v>-0.220232635929218</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.220232635929218</v>
+        <v>-0.130100551073815</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.130100551073815</v>
+        <v>-0.678610977143744</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.678610977143744</v>
+        <v>-0.951604850227953</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.951604850227953</v>
+        <v>-0.668449087733363</v>
       </c>
       <c r="H3" t="n">
-        <v>-0.668449087733363</v>
+        <v>-0.736920201729118</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.736920201729118</v>
+        <v>-0.0708186380420548</v>
       </c>
       <c r="J3" t="n">
-        <v>-0.0708186380420548</v>
+        <v>0.806671746342279</v>
       </c>
       <c r="K3" t="n">
-        <v>0.806671746342279</v>
+        <v>-0.418923448549546</v>
       </c>
       <c r="L3" t="n">
-        <v>-0.418923448549546</v>
+        <v>1.39014296970378</v>
       </c>
       <c r="M3" t="n">
-        <v>1.39014296970378</v>
+        <v>-0.488634396625447</v>
       </c>
       <c r="N3" t="n">
-        <v>-0.488634396625447</v>
+        <v>-0.619971191470381</v>
       </c>
       <c r="O3" t="n">
-        <v>-0.619971191470381</v>
+        <v>-1.04747641165838</v>
       </c>
       <c r="P3" t="n">
-        <v>-1.04747641165838</v>
+        <v>-1.47901635168261</v>
       </c>
       <c r="Q3" t="n">
-        <v>-1.47901635168261</v>
+        <v>-0.119059635480957</v>
       </c>
       <c r="R3" t="n">
-        <v>-0.119059635480957</v>
+        <v>0.346192879547475</v>
       </c>
       <c r="S3" t="n">
-        <v>0.346192879547475</v>
+        <v>-0.714966854199836</v>
       </c>
       <c r="T3" t="n">
-        <v>-0.714966854199836</v>
+        <v>1.10722548840639</v>
       </c>
       <c r="U3" t="n">
-        <v>1.10722548840639</v>
+        <v>-1.07274884302543</v>
       </c>
       <c r="V3" t="n">
-        <v>-1.07274884302543</v>
+        <v>0.0832116334155547</v>
       </c>
       <c r="W3" t="n">
-        <v>0.0832116334155547</v>
-      </c>
-      <c r="X3" t="n">
         <v>0.909407102059476</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
-        <v>119</v>
+      <c r="A4" t="n">
+        <v>-0.986761390406177</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.986761390406177</v>
+        <v>-0.772044012093793</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.772044012093793</v>
+        <v>0.974089981270711</v>
       </c>
       <c r="D4" t="n">
-        <v>0.974089981270711</v>
+        <v>1.05135302009463</v>
       </c>
       <c r="E4" t="n">
-        <v>1.05135302009463</v>
+        <v>1.604593177777</v>
       </c>
       <c r="F4" t="n">
-        <v>1.604593177777</v>
+        <v>0.576975787416958</v>
       </c>
       <c r="G4" t="n">
-        <v>0.576975787416958</v>
+        <v>1.29165471031182</v>
       </c>
       <c r="H4" t="n">
-        <v>1.29165471031182</v>
+        <v>1.51657931504448</v>
       </c>
       <c r="I4" t="n">
-        <v>1.51657931504448</v>
+        <v>0.561867379264542</v>
       </c>
       <c r="J4" t="n">
-        <v>0.561867379264542</v>
+        <v>-0.0814312049293967</v>
       </c>
       <c r="K4" t="n">
-        <v>-0.0814312049293967</v>
+        <v>1.1713407657516</v>
       </c>
       <c r="L4" t="n">
-        <v>1.1713407657516</v>
+        <v>-0.602121991185793</v>
       </c>
       <c r="M4" t="n">
-        <v>-0.602121991185793</v>
+        <v>0.985250634561736</v>
       </c>
       <c r="N4" t="n">
-        <v>0.985250634561736</v>
+        <v>1.02429442096836</v>
       </c>
       <c r="O4" t="n">
-        <v>1.02429442096836</v>
+        <v>1.69756620097136</v>
       </c>
       <c r="P4" t="n">
-        <v>1.69756620097136</v>
+        <v>2.05648417324653</v>
       </c>
       <c r="Q4" t="n">
-        <v>2.05648417324653</v>
+        <v>0.0156747398338641</v>
       </c>
       <c r="R4" t="n">
-        <v>0.0156747398338641</v>
+        <v>0.479630186904212</v>
       </c>
       <c r="S4" t="n">
-        <v>0.479630186904212</v>
+        <v>1.55732102983817</v>
       </c>
       <c r="T4" t="n">
-        <v>1.55732102983817</v>
+        <v>-0.729997454146968</v>
       </c>
       <c r="U4" t="n">
-        <v>-0.729997454146968</v>
+        <v>2.35392265133467</v>
       </c>
       <c r="V4" t="n">
-        <v>2.35392265133467</v>
+        <v>0.0379576527450984</v>
       </c>
       <c r="W4" t="n">
-        <v>0.0379576527450984</v>
-      </c>
-      <c r="X4" t="n">
         <v>-0.181719172844014</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
-        <v>120</v>
+      <c r="A5" t="n">
+        <v>0.135688031108185</v>
       </c>
       <c r="B5" t="n">
-        <v>0.135688031108185</v>
+        <v>1.49450464223431</v>
       </c>
       <c r="C5" t="n">
-        <v>1.49450464223431</v>
+        <v>0.0976357568493115</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0976357568493115</v>
+        <v>-0.188137301189861</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.188137301189861</v>
+        <v>0.282118725980557</v>
       </c>
       <c r="F5" t="n">
-        <v>0.282118725980557</v>
+        <v>0.0758358161710585</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0758358161710585</v>
+        <v>-0.225532053365704</v>
       </c>
       <c r="H5" t="n">
-        <v>-0.225532053365704</v>
+        <v>-0.0769390706409609</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.0769390706409609</v>
+        <v>-0.545216549298544</v>
       </c>
       <c r="J5" t="n">
-        <v>-0.545216549298544</v>
+        <v>0.414723455386916</v>
       </c>
       <c r="K5" t="n">
-        <v>0.414723455386916</v>
+        <v>-0.29335703816155</v>
       </c>
       <c r="L5" t="n">
-        <v>-0.29335703816155</v>
+        <v>2.02487073476144</v>
       </c>
       <c r="M5" t="n">
-        <v>2.02487073476144</v>
+        <v>-0.0693496245178621</v>
       </c>
       <c r="N5" t="n">
-        <v>-0.0693496245178621</v>
+        <v>0.0000678103124660837</v>
       </c>
       <c r="O5" t="n">
-        <v>0.0000678103124660837</v>
+        <v>1.16883233408038</v>
       </c>
       <c r="P5" t="n">
-        <v>1.16883233408038</v>
+        <v>-0.108451336028929</v>
       </c>
       <c r="Q5" t="n">
-        <v>-0.108451336028929</v>
+        <v>-0.529800497361924</v>
       </c>
       <c r="R5" t="n">
-        <v>-0.529800497361924</v>
+        <v>0.607317102240238</v>
       </c>
       <c r="S5" t="n">
-        <v>0.607317102240238</v>
+        <v>0.407230196830939</v>
       </c>
       <c r="T5" t="n">
-        <v>0.407230196830939</v>
+        <v>2.00304274776986</v>
       </c>
       <c r="U5" t="n">
-        <v>2.00304274776986</v>
+        <v>0.300209861197939</v>
       </c>
       <c r="V5" t="n">
-        <v>0.300209861197939</v>
+        <v>-0.944283417926256</v>
       </c>
       <c r="W5" t="n">
-        <v>-0.944283417926256</v>
-      </c>
-      <c r="X5" t="n">
         <v>0.57867935988357</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s">
-        <v>121</v>
+      <c r="A6" t="n">
+        <v>0.0770539733447342</v>
       </c>
       <c r="B6" t="n">
-        <v>0.0770539733447342</v>
+        <v>0.302866400919668</v>
       </c>
       <c r="C6" t="n">
-        <v>0.302866400919668</v>
+        <v>-0.543608283194567</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.543608283194567</v>
+        <v>-0.622092390422354</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.622092390422354</v>
+        <v>-0.371674157594627</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.371674157594627</v>
+        <v>0.0935424165574429</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0935424165574429</v>
+        <v>-0.773833590414737</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.773833590414737</v>
+        <v>-0.238891873975283</v>
       </c>
       <c r="I6" t="n">
-        <v>-0.238891873975283</v>
+        <v>-0.518356726906565</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.518356726906565</v>
+        <v>0.965469451024862</v>
       </c>
       <c r="K6" t="n">
-        <v>0.965469451024862</v>
+        <v>-0.450329848320705</v>
       </c>
       <c r="L6" t="n">
-        <v>-0.450329848320705</v>
+        <v>-0.462336351651963</v>
       </c>
       <c r="M6" t="n">
-        <v>-0.462336351651963</v>
+        <v>-0.451870169126869</v>
       </c>
       <c r="N6" t="n">
-        <v>-0.451870169126869</v>
+        <v>-0.429895527145101</v>
       </c>
       <c r="O6" t="n">
-        <v>-0.429895527145101</v>
+        <v>-0.115398217352912</v>
       </c>
       <c r="P6" t="n">
-        <v>-0.115398217352912</v>
+        <v>-1.17074776527235</v>
       </c>
       <c r="Q6" t="n">
-        <v>-1.17074776527235</v>
+        <v>-0.0282186480166078</v>
       </c>
       <c r="R6" t="n">
-        <v>-0.0282186480166078</v>
+        <v>-0.450143119182933</v>
       </c>
       <c r="S6" t="n">
-        <v>-0.450143119182933</v>
+        <v>-0.0668961705362156</v>
       </c>
       <c r="T6" t="n">
-        <v>-0.0668961705362156</v>
+        <v>-0.0841311171398445</v>
       </c>
       <c r="U6" t="n">
-        <v>-0.0841311171398445</v>
+        <v>-0.822599297549716</v>
       </c>
       <c r="V6" t="n">
-        <v>-0.822599297549716</v>
+        <v>-0.0697523651244699</v>
       </c>
       <c r="W6" t="n">
-        <v>-0.0697523651244699</v>
-      </c>
-      <c r="X6" t="n">
         <v>-0.106454589461453</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s">
-        <v>122</v>
+      <c r="A7" t="n">
+        <v>0.0404947882781174</v>
       </c>
       <c r="B7" t="n">
-        <v>0.0404947882781174</v>
+        <v>-0.414864946813832</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.414864946813832</v>
+        <v>-0.550029577940684</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.550029577940684</v>
+        <v>-0.202125390528597</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.202125390528597</v>
+        <v>-0.19420037184982</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.19420037184982</v>
+        <v>0.360481945102388</v>
       </c>
       <c r="G7" t="n">
-        <v>0.360481945102388</v>
+        <v>0.198902735588543</v>
       </c>
       <c r="H7" t="n">
-        <v>0.198902735588543</v>
+        <v>-0.436059312312254</v>
       </c>
       <c r="I7" t="n">
-        <v>-0.436059312312254</v>
+        <v>0.33187099832582</v>
       </c>
       <c r="J7" t="n">
-        <v>0.33187099832582</v>
+        <v>-0.0276786452588162</v>
       </c>
       <c r="K7" t="n">
-        <v>-0.0276786452588162</v>
+        <v>0.319813084885189</v>
       </c>
       <c r="L7" t="n">
-        <v>0.319813084885189</v>
+        <v>-0.621701855324189</v>
       </c>
       <c r="M7" t="n">
-        <v>-0.621701855324189</v>
+        <v>-0.299058027469004</v>
       </c>
       <c r="N7" t="n">
-        <v>-0.299058027469004</v>
+        <v>-0.27932529002674</v>
       </c>
       <c r="O7" t="n">
-        <v>-0.27932529002674</v>
+        <v>-0.673578198506931</v>
       </c>
       <c r="P7" t="n">
-        <v>-0.673578198506931</v>
+        <v>0.0457403856232626</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.0457403856232626</v>
+        <v>0.690388115633142</v>
       </c>
       <c r="R7" t="n">
-        <v>0.690388115633142</v>
+        <v>-0.24327325241873</v>
       </c>
       <c r="S7" t="n">
-        <v>-0.24327325241873</v>
+        <v>-0.688390957230675</v>
       </c>
       <c r="T7" t="n">
-        <v>-0.688390957230675</v>
+        <v>-0.27353024844425</v>
       </c>
       <c r="U7" t="n">
-        <v>-0.27353024844425</v>
+        <v>-0.715958845414613</v>
       </c>
       <c r="V7" t="n">
-        <v>-0.715958845414613</v>
+        <v>1.20150507818257</v>
       </c>
       <c r="W7" t="n">
-        <v>1.20150507818257</v>
-      </c>
-      <c r="X7" t="n">
         <v>-0.00474022315537953</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="s">
-        <v>123</v>
+      <c r="A8" t="n">
+        <v>0.233917569677791</v>
       </c>
       <c r="B8" t="n">
-        <v>0.233917569677791</v>
+        <v>0.515471420320347</v>
       </c>
       <c r="C8" t="n">
-        <v>0.515471420320347</v>
+        <v>0.0175194910141728</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0175194910141728</v>
+        <v>-0.349484440304065</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.349484440304065</v>
+        <v>-0.386045205427395</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.386045205427395</v>
+        <v>-0.132722981608746</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.132722981608746</v>
+        <v>-0.490856712224145</v>
       </c>
       <c r="H8" t="n">
-        <v>-0.490856712224145</v>
+        <v>-0.435661699754898</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.435661699754898</v>
+        <v>0.00187758403215112</v>
       </c>
       <c r="J8" t="n">
-        <v>0.00187758403215112</v>
+        <v>-0.317804427028122</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.317804427028122</v>
+        <v>-0.281955876635323</v>
       </c>
       <c r="L8" t="n">
-        <v>-0.281955876635323</v>
+        <v>0.317354110589388</v>
       </c>
       <c r="M8" t="n">
-        <v>0.317354110589388</v>
+        <v>-0.307610360655606</v>
       </c>
       <c r="N8" t="n">
-        <v>-0.307610360655606</v>
+        <v>-0.256221081712159</v>
       </c>
       <c r="O8" t="n">
-        <v>-0.256221081712159</v>
+        <v>-0.637193249610474</v>
       </c>
       <c r="P8" t="n">
-        <v>-0.637193249610474</v>
+        <v>-0.250322246252809</v>
       </c>
       <c r="Q8" t="n">
-        <v>-0.250322246252809</v>
+        <v>-0.0283271227076605</v>
       </c>
       <c r="R8" t="n">
-        <v>-0.0283271227076605</v>
+        <v>0.186103595560284</v>
       </c>
       <c r="S8" t="n">
-        <v>0.186103595560284</v>
+        <v>-0.247836497742732</v>
       </c>
       <c r="T8" t="n">
-        <v>-0.247836497742732</v>
+        <v>0.349563457904469</v>
       </c>
       <c r="U8" t="n">
-        <v>0.349563457904469</v>
+        <v>-0.421963532837897</v>
       </c>
       <c r="V8" t="n">
-        <v>-0.421963532837897</v>
+        <v>-0.333318532719887</v>
       </c>
       <c r="W8" t="n">
-        <v>-0.333318532719887</v>
-      </c>
-      <c r="X8" t="n">
         <v>0.0455477488219248</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="s">
-        <v>124</v>
+      <c r="A9" t="n">
+        <v>-0.465745865029967</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.465745865029967</v>
+        <v>-0.2499908690813</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.2499908690813</v>
+        <v>-0.523146901586802</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.523146901586802</v>
+        <v>-0.382605772579067</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.382605772579067</v>
+        <v>-0.401096887363094</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.401096887363094</v>
+        <v>1.23067669727648</v>
       </c>
       <c r="G9" t="n">
-        <v>1.23067669727648</v>
+        <v>-0.326588292719027</v>
       </c>
       <c r="H9" t="n">
-        <v>-0.326588292719027</v>
+        <v>-0.476866432720395</v>
       </c>
       <c r="I9" t="n">
-        <v>-0.476866432720395</v>
+        <v>-0.746585733035012</v>
       </c>
       <c r="J9" t="n">
-        <v>-0.746585733035012</v>
+        <v>-0.604990942230045</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.604990942230045</v>
+        <v>-0.555347965591385</v>
       </c>
       <c r="L9" t="n">
-        <v>-0.555347965591385</v>
+        <v>0.28206957720551</v>
       </c>
       <c r="M9" t="n">
-        <v>0.28206957720551</v>
+        <v>-0.495274136583367</v>
       </c>
       <c r="N9" t="n">
-        <v>-0.495274136583367</v>
+        <v>-0.175167885440641</v>
       </c>
       <c r="O9" t="n">
-        <v>-0.175167885440641</v>
+        <v>-0.375201162214969</v>
       </c>
       <c r="P9" t="n">
-        <v>-0.375201162214969</v>
+        <v>-0.27532536379984</v>
       </c>
       <c r="Q9" t="n">
-        <v>-0.27532536379984</v>
+        <v>-0.108285720636435</v>
       </c>
       <c r="R9" t="n">
-        <v>-0.108285720636435</v>
+        <v>-0.755554641409861</v>
       </c>
       <c r="S9" t="n">
-        <v>-0.755554641409861</v>
+        <v>-0.533973774913479</v>
       </c>
       <c r="T9" t="n">
-        <v>-0.533973774913479</v>
+        <v>-0.130053758599217</v>
       </c>
       <c r="U9" t="n">
-        <v>-0.130053758599217</v>
+        <v>-0.470142474233395</v>
       </c>
       <c r="V9" t="n">
-        <v>-0.470142474233395</v>
+        <v>-0.59760434877578</v>
       </c>
       <c r="W9" t="n">
-        <v>-0.59760434877578</v>
-      </c>
-      <c r="X9" t="n">
         <v>-0.62420995411974</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s">
-        <v>125</v>
+      <c r="A10" t="n">
+        <v>0.345911669571026</v>
       </c>
       <c r="B10" t="n">
-        <v>0.345911669571026</v>
+        <v>-1.03329301267967</v>
       </c>
       <c r="C10" t="n">
-        <v>-1.03329301267967</v>
+        <v>-0.405759961565337</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.405759961565337</v>
+        <v>-0.186141639941228</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.186141639941228</v>
+        <v>-0.396506514524694</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.396506514524694</v>
+        <v>-0.68773868429233</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.68773868429233</v>
+        <v>0.256595210123654</v>
       </c>
       <c r="H10" t="n">
-        <v>0.256595210123654</v>
+        <v>-0.377445873253773</v>
       </c>
       <c r="I10" t="n">
-        <v>-0.377445873253773</v>
+        <v>-0.19230305466677</v>
       </c>
       <c r="J10" t="n">
-        <v>-0.19230305466677</v>
+        <v>-0.388814598292494</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.388814598292494</v>
+        <v>-0.243835876051517</v>
       </c>
       <c r="L10" t="n">
-        <v>-0.243835876051517</v>
+        <v>-1.00446557509809</v>
       </c>
       <c r="M10" t="n">
-        <v>-1.00446557509809</v>
+        <v>0.111306023171069</v>
       </c>
       <c r="N10" t="n">
-        <v>0.111306023171069</v>
+        <v>-0.250222112844393</v>
       </c>
       <c r="O10" t="n">
-        <v>-0.250222112844393</v>
+        <v>-0.138704437002629</v>
       </c>
       <c r="P10" t="n">
-        <v>-0.138704437002629</v>
+        <v>0.216915663236609</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.216915663236609</v>
+        <v>0.0784187222832774</v>
       </c>
       <c r="R10" t="n">
-        <v>0.0784187222832774</v>
+        <v>-0.439531273745602</v>
       </c>
       <c r="S10" t="n">
-        <v>-0.439531273745602</v>
+        <v>-0.535454755478304</v>
       </c>
       <c r="T10" t="n">
-        <v>-0.535454755478304</v>
+        <v>-0.787326011992009</v>
       </c>
       <c r="U10" t="n">
-        <v>-0.787326011992009</v>
+        <v>-0.463467599919065</v>
       </c>
       <c r="V10" t="n">
-        <v>-0.463467599919065</v>
+        <v>0.30183090866006</v>
       </c>
       <c r="W10" t="n">
-        <v>0.30183090866006</v>
-      </c>
-      <c r="X10" t="n">
         <v>-0.30435700935969</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s">
-        <v>23</v>
+      <c r="A11" t="n">
+        <v>-0.593846267368161</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.593846267368161</v>
+        <v>-1.15414279081911</v>
       </c>
       <c r="C11" t="n">
-        <v>-1.15414279081911</v>
+        <v>0.998990577241354</v>
       </c>
       <c r="D11" t="n">
-        <v>0.998990577241354</v>
+        <v>1.05681282892511</v>
       </c>
       <c r="E11" t="n">
-        <v>1.05681282892511</v>
+        <v>0.596669068673392</v>
       </c>
       <c r="F11" t="n">
-        <v>0.596669068673392</v>
+        <v>-0.595390525450417</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.595390525450417</v>
+        <v>0.7703244841088</v>
       </c>
       <c r="H11" t="n">
-        <v>0.7703244841088</v>
+        <v>1.20676729504782</v>
       </c>
       <c r="I11" t="n">
-        <v>1.20676729504782</v>
+        <v>1.34117651426268</v>
       </c>
       <c r="J11" t="n">
-        <v>1.34117651426268</v>
+        <v>-0.0881588100492298</v>
       </c>
       <c r="K11" t="n">
-        <v>-0.0881588100492298</v>
+        <v>0.960811764156139</v>
       </c>
       <c r="L11" t="n">
-        <v>0.960811764156139</v>
+        <v>-1.20180605404257</v>
       </c>
       <c r="M11" t="n">
-        <v>-1.20180605404257</v>
+        <v>0.930750035417141</v>
       </c>
       <c r="N11" t="n">
-        <v>0.930750035417141</v>
+        <v>0.869075419603146</v>
       </c>
       <c r="O11" t="n">
-        <v>0.869075419603146</v>
+        <v>0.0794820990614283</v>
       </c>
       <c r="P11" t="n">
-        <v>0.0794820990614283</v>
+        <v>0.60793121771483</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.60793121771483</v>
+        <v>0.294458311327927</v>
       </c>
       <c r="R11" t="n">
-        <v>0.294458311327927</v>
+        <v>0.39402647714176</v>
       </c>
       <c r="S11" t="n">
-        <v>0.39402647714176</v>
+        <v>0.723846022331551</v>
       </c>
       <c r="T11" t="n">
-        <v>0.723846022331551</v>
+        <v>-1.27193493907841</v>
       </c>
       <c r="U11" t="n">
-        <v>-1.27193493907841</v>
+        <v>1.03180538097325</v>
       </c>
       <c r="V11" t="n">
-        <v>1.03180538097325</v>
+        <v>0.933270914272267</v>
       </c>
       <c r="W11" t="n">
-        <v>0.933270914272267</v>
-      </c>
-      <c r="X11" t="n">
         <v>0.0808862506754261</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="s">
-        <v>126</v>
+      <c r="A12" t="n">
+        <v>-0.753265289843352</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.753265289843352</v>
+        <v>-0.791588888631569</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.791588888631569</v>
+        <v>0.957609756671358</v>
       </c>
       <c r="D12" t="n">
-        <v>0.957609756671358</v>
+        <v>0.437698364532612</v>
       </c>
       <c r="E12" t="n">
-        <v>0.437698364532612</v>
+        <v>0.862998241715303</v>
       </c>
       <c r="F12" t="n">
-        <v>0.862998241715303</v>
+        <v>-0.661442096531054</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.661442096531054</v>
+        <v>-0.773223588730698</v>
       </c>
       <c r="H12" t="n">
-        <v>-0.773223588730698</v>
+        <v>1.41822816983595</v>
       </c>
       <c r="I12" t="n">
-        <v>1.41822816983595</v>
+        <v>0.742946347015174</v>
       </c>
       <c r="J12" t="n">
-        <v>0.742946347015174</v>
+        <v>-0.752222956623928</v>
       </c>
       <c r="K12" t="n">
-        <v>-0.752222956623928</v>
+        <v>0.1323415504395</v>
       </c>
       <c r="L12" t="n">
-        <v>0.1323415504395</v>
+        <v>-0.803215969096286</v>
       </c>
       <c r="M12" t="n">
-        <v>-0.803215969096286</v>
+        <v>-0.493833001348481</v>
       </c>
       <c r="N12" t="n">
-        <v>-0.493833001348481</v>
+        <v>0.404717660976818</v>
       </c>
       <c r="O12" t="n">
-        <v>0.404717660976818</v>
+        <v>-0.77193424762943</v>
       </c>
       <c r="P12" t="n">
-        <v>-0.77193424762943</v>
+        <v>2.09650931336335</v>
       </c>
       <c r="Q12" t="n">
-        <v>2.09650931336335</v>
+        <v>-0.533018976310836</v>
       </c>
       <c r="R12" t="n">
-        <v>-0.533018976310836</v>
+        <v>0.943285805333189</v>
       </c>
       <c r="S12" t="n">
-        <v>0.943285805333189</v>
+        <v>0.88340851603469</v>
       </c>
       <c r="T12" t="n">
-        <v>0.88340851603469</v>
+        <v>-0.738082653477906</v>
       </c>
       <c r="U12" t="n">
-        <v>-0.738082653477906</v>
+        <v>-0.414336128779038</v>
       </c>
       <c r="V12" t="n">
-        <v>-0.414336128779038</v>
+        <v>-0.794647627797327</v>
       </c>
       <c r="W12" t="n">
-        <v>-0.794647627797327</v>
-      </c>
-      <c r="X12" t="n">
         <v>-0.79563292185626</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="s">
-        <v>127</v>
+      <c r="A13" t="n">
+        <v>-0.575551396360498</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.575551396360498</v>
+        <v>-0.646793349048476</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.646793349048476</v>
+        <v>0.507786831736535</v>
       </c>
       <c r="D13" t="n">
-        <v>0.507786831736535</v>
+        <v>2.33472417593212</v>
       </c>
       <c r="E13" t="n">
-        <v>2.33472417593212</v>
+        <v>1.29272186315313</v>
       </c>
       <c r="F13" t="n">
-        <v>1.29272186315313</v>
+        <v>0.127351894897867</v>
       </c>
       <c r="G13" t="n">
-        <v>0.127351894897867</v>
+        <v>-0.901145965905741</v>
       </c>
       <c r="H13" t="n">
-        <v>-0.901145965905741</v>
+        <v>0.467603824671809</v>
       </c>
       <c r="I13" t="n">
-        <v>0.467603824671809</v>
+        <v>0.657900790574586</v>
       </c>
       <c r="J13" t="n">
-        <v>0.657900790574586</v>
+        <v>0.0032767656540103</v>
       </c>
       <c r="K13" t="n">
-        <v>0.0032767656540103</v>
+        <v>1.95368717217853</v>
       </c>
       <c r="L13" t="n">
-        <v>1.95368717217853</v>
+        <v>-0.842924480205492</v>
       </c>
       <c r="M13" t="n">
-        <v>-0.842924480205492</v>
+        <v>0.808126234735768</v>
       </c>
       <c r="N13" t="n">
-        <v>0.808126234735768</v>
+        <v>0.863119369272829</v>
       </c>
       <c r="O13" t="n">
-        <v>0.863119369272829</v>
+        <v>-0.879820735538346</v>
       </c>
       <c r="P13" t="n">
-        <v>-0.879820735538346</v>
+        <v>-0.414851011182359</v>
       </c>
       <c r="Q13" t="n">
-        <v>-0.414851011182359</v>
+        <v>-0.70191546898585</v>
       </c>
       <c r="R13" t="n">
-        <v>-0.70191546898585</v>
+        <v>1.00259321231163</v>
       </c>
       <c r="S13" t="n">
-        <v>1.00259321231163</v>
+        <v>-0.24356047140334</v>
       </c>
       <c r="T13" t="n">
-        <v>-0.24356047140334</v>
+        <v>-0.801242547918978</v>
       </c>
       <c r="U13" t="n">
-        <v>-0.801242547918978</v>
+        <v>-0.544968738505398</v>
       </c>
       <c r="V13" t="n">
-        <v>-0.544968738505398</v>
+        <v>-0.985476965398001</v>
       </c>
       <c r="W13" t="n">
-        <v>-0.985476965398001</v>
-      </c>
-      <c r="X13" t="n">
         <v>-0.919687357008204</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="s">
-        <v>128</v>
+      <c r="A14" t="n">
+        <v>-0.205734423789736</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.205734423789736</v>
+        <v>0.870982793371001</v>
       </c>
       <c r="C14" t="n">
-        <v>0.870982793371001</v>
+        <v>0.129596335797766</v>
       </c>
       <c r="D14" t="n">
-        <v>0.129596335797766</v>
+        <v>-0.530890946522053</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.530890946522053</v>
+        <v>-0.0219976578598537</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.0219976578598537</v>
+        <v>1.55217489105105</v>
       </c>
       <c r="G14" t="n">
-        <v>1.55217489105105</v>
+        <v>-0.725760807071407</v>
       </c>
       <c r="H14" t="n">
-        <v>-0.725760807071407</v>
+        <v>-0.51746363497366</v>
       </c>
       <c r="I14" t="n">
-        <v>-0.51746363497366</v>
+        <v>-0.0176958391691852</v>
       </c>
       <c r="J14" t="n">
-        <v>-0.0176958391691852</v>
+        <v>1.13280383417234</v>
       </c>
       <c r="K14" t="n">
-        <v>1.13280383417234</v>
+        <v>0.0190378386876468</v>
       </c>
       <c r="L14" t="n">
-        <v>0.0190378386876468</v>
+        <v>-0.580966179555527</v>
       </c>
       <c r="M14" t="n">
-        <v>-0.580966179555527</v>
+        <v>0.622234040738586</v>
       </c>
       <c r="N14" t="n">
-        <v>0.622234040738586</v>
+        <v>0.0890140401562253</v>
       </c>
       <c r="O14" t="n">
-        <v>0.0890140401562253</v>
+        <v>-0.0285723393823273</v>
       </c>
       <c r="P14" t="n">
-        <v>-0.0285723393823273</v>
+        <v>-0.393713187402756</v>
       </c>
       <c r="Q14" t="n">
-        <v>-0.393713187402756</v>
+        <v>-0.723169081514</v>
       </c>
       <c r="R14" t="n">
-        <v>-0.723169081514</v>
+        <v>-0.531537970216421</v>
       </c>
       <c r="S14" t="n">
-        <v>-0.531537970216421</v>
+        <v>-0.638880838757158</v>
       </c>
       <c r="T14" t="n">
-        <v>-0.638880838757158</v>
+        <v>-0.576387857934643</v>
       </c>
       <c r="U14" t="n">
-        <v>-0.576387857934643</v>
+        <v>-0.534815747614707</v>
       </c>
       <c r="V14" t="n">
-        <v>-0.534815747614707</v>
+        <v>-0.870031073821448</v>
       </c>
       <c r="W14" t="n">
-        <v>-0.870031073821448</v>
-      </c>
-      <c r="X14" t="n">
         <v>-0.0696761634730108</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="s">
-        <v>129</v>
+      <c r="A15" t="n">
+        <v>-0.0444900805219199</v>
       </c>
       <c r="B15" t="n">
-        <v>-0.0444900805219199</v>
+        <v>-0.626580324170176</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.626580324170176</v>
+        <v>0.139015530391162</v>
       </c>
       <c r="D15" t="n">
-        <v>0.139015530391162</v>
+        <v>0.122368608608379</v>
       </c>
       <c r="E15" t="n">
-        <v>0.122368608608379</v>
+        <v>-0.532005296955358</v>
       </c>
       <c r="F15" t="n">
-        <v>-0.532005296955358</v>
+        <v>0.382125072651379</v>
       </c>
       <c r="G15" t="n">
-        <v>0.382125072651379</v>
+        <v>1.20335025107636</v>
       </c>
       <c r="H15" t="n">
-        <v>1.20335025107636</v>
+        <v>0.324186851998935</v>
       </c>
       <c r="I15" t="n">
-        <v>0.324186851998935</v>
+        <v>-0.2679349630077</v>
       </c>
       <c r="J15" t="n">
-        <v>-0.2679349630077</v>
+        <v>-0.742637008541527</v>
       </c>
       <c r="K15" t="n">
-        <v>-0.742637008541527</v>
+        <v>0.227313993572846</v>
       </c>
       <c r="L15" t="n">
-        <v>0.227313993572846</v>
+        <v>-0.692009713828217</v>
       </c>
       <c r="M15" t="n">
-        <v>-0.692009713828217</v>
+        <v>1.63616277162404</v>
       </c>
       <c r="N15" t="n">
-        <v>1.63616277162404</v>
+        <v>-0.521461362343701</v>
       </c>
       <c r="O15" t="n">
-        <v>-0.521461362343701</v>
+        <v>0.366329765453922</v>
       </c>
       <c r="P15" t="n">
-        <v>0.366329765453922</v>
+        <v>-0.387954369046413</v>
       </c>
       <c r="Q15" t="n">
-        <v>-0.387954369046413</v>
+        <v>2.33497232079654</v>
       </c>
       <c r="R15" t="n">
-        <v>2.33497232079654</v>
+        <v>-0.497012108866951</v>
       </c>
       <c r="S15" t="n">
-        <v>-0.497012108866951</v>
+        <v>0.773098013141497</v>
       </c>
       <c r="T15" t="n">
-        <v>0.773098013141497</v>
+        <v>-0.705764799494448</v>
       </c>
       <c r="U15" t="n">
-        <v>-0.705764799494448</v>
+        <v>1.63785660294322</v>
       </c>
       <c r="V15" t="n">
-        <v>1.63785660294322</v>
+        <v>2.43522573435228</v>
       </c>
       <c r="W15" t="n">
-        <v>2.43522573435228</v>
-      </c>
-      <c r="X15" t="n">
         <v>-0.690535415278506</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="s">
-        <v>130</v>
+      <c r="A16" t="n">
+        <v>0.0894019623800398</v>
       </c>
       <c r="B16" t="n">
-        <v>0.0894019623800398</v>
+        <v>0.90187406248223</v>
       </c>
       <c r="C16" t="n">
-        <v>0.90187406248223</v>
+        <v>-0.802758891834407</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.802758891834407</v>
+        <v>-0.675112897339848</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.675112897339848</v>
+        <v>-0.681297072238712</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.681297072238712</v>
+        <v>1.20696410799265</v>
       </c>
       <c r="G16" t="n">
-        <v>1.20696410799265</v>
+        <v>2.25160615149497</v>
       </c>
       <c r="H16" t="n">
-        <v>2.25160615149497</v>
+        <v>-0.529309040136736</v>
       </c>
       <c r="I16" t="n">
-        <v>-0.529309040136736</v>
+        <v>-0.475144747089425</v>
       </c>
       <c r="J16" t="n">
-        <v>-0.475144747089425</v>
+        <v>0.707131298751438</v>
       </c>
       <c r="K16" t="n">
-        <v>0.707131298751438</v>
+        <v>-0.204839696657985</v>
       </c>
       <c r="L16" t="n">
-        <v>-0.204839696657985</v>
+        <v>0.38030389757025</v>
       </c>
       <c r="M16" t="n">
-        <v>0.38030389757025</v>
+        <v>-0.615962016210663</v>
       </c>
       <c r="N16" t="n">
-        <v>-0.615962016210663</v>
+        <v>-0.420657321900764</v>
       </c>
       <c r="O16" t="n">
-        <v>-0.420657321900764</v>
+        <v>2.47712190322863</v>
       </c>
       <c r="P16" t="n">
-        <v>2.47712190322863</v>
+        <v>-0.765851701117687</v>
       </c>
       <c r="Q16" t="n">
-        <v>-0.765851701117687</v>
+        <v>-0.178098541186874</v>
       </c>
       <c r="R16" t="n">
-        <v>-0.178098541186874</v>
+        <v>-0.493097087701602</v>
       </c>
       <c r="S16" t="n">
-        <v>-0.493097087701602</v>
+        <v>-0.63904602406547</v>
       </c>
       <c r="T16" t="n">
-        <v>-0.63904602406547</v>
+        <v>0.475266302219576</v>
       </c>
       <c r="U16" t="n">
-        <v>0.475266302219576</v>
+        <v>-0.379219344898934</v>
       </c>
       <c r="V16" t="n">
-        <v>-0.379219344898934</v>
+        <v>-0.580045479112795</v>
       </c>
       <c r="W16" t="n">
-        <v>-0.580045479112795</v>
-      </c>
-      <c r="X16" t="n">
         <v>-0.475564655229996</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="s">
-        <v>131</v>
+      <c r="A17" t="n">
+        <v>-0.129137395127345</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.129137395127345</v>
+        <v>-0.245281255939389</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.245281255939389</v>
+        <v>-0.319456439820845</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.319456439820845</v>
+        <v>-0.321374071106152</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.321374071106152</v>
+        <v>-0.313951080534249</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.313951080534249</v>
+        <v>-0.178326355390406</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.178326355390406</v>
+        <v>0.0741798703001086</v>
       </c>
       <c r="H17" t="n">
-        <v>0.0741798703001086</v>
+        <v>-0.307928359181948</v>
       </c>
       <c r="I17" t="n">
-        <v>-0.307928359181948</v>
+        <v>-0.290496297771228</v>
       </c>
       <c r="J17" t="n">
-        <v>-0.290496297771228</v>
+        <v>0.326334467880177</v>
       </c>
       <c r="K17" t="n">
-        <v>0.326334467880177</v>
+        <v>-0.308265489025616</v>
       </c>
       <c r="L17" t="n">
-        <v>-0.308265489025616</v>
+        <v>-0.00586129715888197</v>
       </c>
       <c r="M17" t="n">
-        <v>-0.00586129715888197</v>
+        <v>-0.316718843605564</v>
       </c>
       <c r="N17" t="n">
-        <v>-0.316718843605564</v>
+        <v>-0.161733019968742</v>
       </c>
       <c r="O17" t="n">
-        <v>-0.161733019968742</v>
+        <v>-0.251744028003077</v>
       </c>
       <c r="P17" t="n">
-        <v>-0.251744028003077</v>
+        <v>-0.303160793498876</v>
       </c>
       <c r="Q17" t="n">
-        <v>-0.303160793498876</v>
+        <v>-0.284113117857983</v>
       </c>
       <c r="R17" t="n">
-        <v>-0.284113117857983</v>
+        <v>-0.289932757371378</v>
       </c>
       <c r="S17" t="n">
-        <v>-0.289932757371378</v>
+        <v>-0.318383885769756</v>
       </c>
       <c r="T17" t="n">
-        <v>-0.318383885769756</v>
+        <v>0.393425795089351</v>
       </c>
       <c r="U17" t="n">
-        <v>0.393425795089351</v>
+        <v>0.122509630753378</v>
       </c>
       <c r="V17" t="n">
-        <v>0.122509630753378</v>
+        <v>1.34410325053068</v>
       </c>
       <c r="W17" t="n">
-        <v>1.34410325053068</v>
-      </c>
-      <c r="X17" t="n">
         <v>0.976908679655748</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="s">
-        <v>132</v>
+      <c r="A18" t="n">
+        <v>-0.461719464901485</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.461719464901485</v>
+        <v>-0.443212011398654</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.443212011398654</v>
+        <v>-0.52577700593981</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.52577700593981</v>
+        <v>-0.525908312086709</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.525908312086709</v>
+        <v>-0.517035463720882</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.517035463720882</v>
+        <v>-0.507989334221928</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.507989334221928</v>
+        <v>-0.0439912075210081</v>
       </c>
       <c r="H18" t="n">
-        <v>-0.0439912075210081</v>
+        <v>-0.468732627432272</v>
       </c>
       <c r="I18" t="n">
-        <v>-0.468732627432272</v>
+        <v>-0.121222359679859</v>
       </c>
       <c r="J18" t="n">
-        <v>-0.121222359679859</v>
+        <v>0.242200241791388</v>
       </c>
       <c r="K18" t="n">
-        <v>0.242200241791388</v>
+        <v>-0.373734634308963</v>
       </c>
       <c r="L18" t="n">
-        <v>-0.373734634308963</v>
+        <v>1.95368516456214</v>
       </c>
       <c r="M18" t="n">
-        <v>1.95368516456214</v>
+        <v>-0.524517711539196</v>
       </c>
       <c r="N18" t="n">
-        <v>-0.524517711539196</v>
+        <v>-0.288497469895774</v>
       </c>
       <c r="O18" t="n">
-        <v>-0.288497469895774</v>
+        <v>0.0159393682196303</v>
       </c>
       <c r="P18" t="n">
-        <v>0.0159393682196303</v>
+        <v>-0.282159704667895</v>
       </c>
       <c r="Q18" t="n">
-        <v>-0.282159704667895</v>
+        <v>-0.502107806612864</v>
       </c>
       <c r="R18" t="n">
-        <v>-0.502107806612864</v>
+        <v>-0.514343867902819</v>
       </c>
       <c r="S18" t="n">
-        <v>-0.514343867902819</v>
+        <v>-0.52217738356536</v>
       </c>
       <c r="T18" t="n">
-        <v>-0.52217738356536</v>
+        <v>1.82059587713102</v>
       </c>
       <c r="U18" t="n">
-        <v>1.82059587713102</v>
+        <v>-0.491676587343349</v>
       </c>
       <c r="V18" t="n">
-        <v>-0.491676587343349</v>
+        <v>-0.458178581560971</v>
       </c>
       <c r="W18" t="n">
-        <v>-0.458178581560971</v>
-      </c>
-      <c r="X18" t="n">
         <v>1.16119672402963</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="s">
-        <v>133</v>
+      <c r="A19" t="n">
+        <v>1.19267706091775</v>
       </c>
       <c r="B19" t="n">
-        <v>1.19267706091775</v>
+        <v>-0.301052525341922</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.301052525341922</v>
+        <v>0.400086440006511</v>
       </c>
       <c r="D19" t="n">
-        <v>0.400086440006511</v>
+        <v>0.752966900840336</v>
       </c>
       <c r="E19" t="n">
-        <v>0.752966900840336</v>
+        <v>0.739135356142898</v>
       </c>
       <c r="F19" t="n">
-        <v>0.739135356142898</v>
+        <v>-1.07487700452682</v>
       </c>
       <c r="G19" t="n">
-        <v>-1.07487700452682</v>
+        <v>0.0975570138874772</v>
       </c>
       <c r="H19" t="n">
-        <v>0.0975570138874772</v>
+        <v>-0.0940086036329307</v>
       </c>
       <c r="I19" t="n">
-        <v>-0.0940086036329307</v>
+        <v>-0.295805526537364</v>
       </c>
       <c r="J19" t="n">
-        <v>-0.295805526537364</v>
+        <v>-0.170151998725486</v>
       </c>
       <c r="K19" t="n">
-        <v>-0.170151998725486</v>
+        <v>-0.298365811858222</v>
       </c>
       <c r="L19" t="n">
-        <v>-0.298365811858222</v>
+        <v>0.0659726205263397</v>
       </c>
       <c r="M19" t="n">
-        <v>0.0659726205263397</v>
+        <v>-0.680706980884602</v>
       </c>
       <c r="N19" t="n">
-        <v>-0.680706980884602</v>
+        <v>0.731435671047399</v>
       </c>
       <c r="O19" t="n">
-        <v>0.731435671047399</v>
+        <v>-0.629644603624357</v>
       </c>
       <c r="P19" t="n">
-        <v>-0.629644603624357</v>
+        <v>0.504763410749726</v>
       </c>
       <c r="Q19" t="n">
-        <v>0.504763410749726</v>
+        <v>1.19942050992602</v>
       </c>
       <c r="R19" t="n">
-        <v>1.19942050992602</v>
+        <v>0.764445140722727</v>
       </c>
       <c r="S19" t="n">
-        <v>0.764445140722727</v>
+        <v>1.08579046865762</v>
       </c>
       <c r="T19" t="n">
-        <v>1.08579046865762</v>
+        <v>-0.364875457478697</v>
       </c>
       <c r="U19" t="n">
-        <v>-0.364875457478697</v>
+        <v>0.529816936057543</v>
       </c>
       <c r="V19" t="n">
-        <v>0.529816936057543</v>
+        <v>-0.138481719341181</v>
       </c>
       <c r="W19" t="n">
-        <v>-0.138481719341181</v>
-      </c>
-      <c r="X19" t="n">
         <v>-0.10087137914155</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="s">
-        <v>134</v>
+      <c r="A20" t="n">
+        <v>1.55915149151557</v>
       </c>
       <c r="B20" t="n">
-        <v>1.55915149151557</v>
+        <v>1.51178286295268</v>
       </c>
       <c r="C20" t="n">
-        <v>1.51178286295268</v>
+        <v>-0.766462374315664</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.766462374315664</v>
+        <v>-1.12500739453955</v>
       </c>
       <c r="E20" t="n">
-        <v>-1.12500739453955</v>
+        <v>-0.686614833628492</v>
       </c>
       <c r="F20" t="n">
-        <v>-0.686614833628492</v>
+        <v>-0.793447341538777</v>
       </c>
       <c r="G20" t="n">
-        <v>-0.793447341538777</v>
+        <v>-0.503472638082524</v>
       </c>
       <c r="H20" t="n">
-        <v>-0.503472638082524</v>
+        <v>-0.901988217179735</v>
       </c>
       <c r="I20" t="n">
-        <v>-0.901988217179735</v>
+        <v>-0.316814936448309</v>
       </c>
       <c r="J20" t="n">
-        <v>-0.316814936448309</v>
+        <v>-0.294968486980585</v>
       </c>
       <c r="K20" t="n">
-        <v>-0.294968486980585</v>
+        <v>-1.01522515708039</v>
       </c>
       <c r="L20" t="n">
-        <v>-1.01522515708039</v>
+        <v>0.840194781016257</v>
       </c>
       <c r="M20" t="n">
-        <v>0.840194781016257</v>
+        <v>-0.709857796440463</v>
       </c>
       <c r="N20" t="n">
-        <v>-0.709857796440463</v>
+        <v>-0.408428270177506</v>
       </c>
       <c r="O20" t="n">
-        <v>-0.408428270177506</v>
+        <v>0.132602633438499</v>
       </c>
       <c r="P20" t="n">
-        <v>0.132602633438499</v>
+        <v>-0.806939461985724</v>
       </c>
       <c r="Q20" t="n">
-        <v>-0.806939461985724</v>
+        <v>-0.234940129843345</v>
       </c>
       <c r="R20" t="n">
-        <v>-0.234940129843345</v>
+        <v>-0.275689548793253</v>
       </c>
       <c r="S20" t="n">
-        <v>-0.275689548793253</v>
+        <v>-0.469835173122079</v>
       </c>
       <c r="T20" t="n">
-        <v>-0.469835173122079</v>
+        <v>0.646800454142474</v>
       </c>
       <c r="U20" t="n">
-        <v>0.646800454142474</v>
+        <v>0.13496023829927</v>
       </c>
       <c r="V20" t="n">
-        <v>0.13496023829927</v>
+        <v>-0.194702699889872</v>
       </c>
       <c r="W20" t="n">
-        <v>-0.194702699889872</v>
-      </c>
-      <c r="X20" t="n">
         <v>0.931326995681454</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update mutational signatures heatmap and tables
</commit_message>
<xml_diff>
--- a/tables/mutational_signatures.xlsx
+++ b/tables/mutational_signatures.xlsx
@@ -8,12 +8,13 @@
   <sheets>
     <sheet name="Mutational signatures" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Signature proportions" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Std signature proportions" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="133">
   <si>
     <t xml:space="preserve">patient_id</t>
   </si>
@@ -294,73 +295,124 @@
     <t xml:space="preserve">SPECTRUM-OV-123</t>
   </si>
   <si>
-    <t xml:space="preserve">063</t>
-  </si>
-  <si>
-    <t xml:space="preserve">067</t>
-  </si>
-  <si>
-    <t xml:space="preserve">028</t>
-  </si>
-  <si>
-    <t xml:space="preserve">003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">031</t>
-  </si>
-  <si>
-    <t xml:space="preserve">045</t>
-  </si>
-  <si>
-    <t xml:space="preserve">036</t>
-  </si>
-  <si>
-    <t xml:space="preserve">007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">044</t>
-  </si>
-  <si>
-    <t xml:space="preserve">026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">054</t>
-  </si>
-  <si>
-    <t xml:space="preserve">053</t>
-  </si>
-  <si>
-    <t xml:space="preserve">049</t>
-  </si>
-  <si>
-    <t xml:space="preserve">051</t>
-  </si>
-  <si>
-    <t xml:space="preserve">050</t>
-  </si>
-  <si>
-    <t xml:space="preserve">025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">068</t>
-  </si>
-  <si>
-    <t xml:space="preserve">082</t>
-  </si>
-  <si>
-    <t xml:space="preserve">083</t>
+    <t xml:space="preserve">topic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPECTRUM-OV-067_S1_INFRACOLIC_OMENTUM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPECTRUM-OV-003_S2_PELVIC_PERITONEUM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPECTRUM-OV-031_S1_LEFT_INFRARENAL_LYMPH_NODE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPECTRUM-OV-045_S1_INFRACOLIC_OMENTUM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPECTRUM-OV-036_S1_BOWEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPECTRUM-OV-007_S1_INFRACOLIC_OMENTUM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPECTRUM-OV-009_S1_RIGHT_OVARY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPECTRUM-OV-026_S1_LIVER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPECTRUM-OV-054_S1_INFRACOLIC_OMENTUM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPECTRUM-OV-053_S1_INFRACOLIC_OMENTUM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPECTRUM-OV-049_S1_COLON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPECTRUM-OV-051_S1_INFRACOLIC_OMENTUM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPECTRUM-OV-050_S1_INFRACOLIC_OMENTUM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPECTRUM-OV-025_S1_RECTUM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPECTRUM-OV-022_S1_LEFT_OVARY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPECTRUM-OV-008_S1_LEFT_RENAL_LYMPH_NODE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPECTRUM-OV-002_S1_INFRACOLIC_OMENTUM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPECTRUM-OV-068_S1_INFRACOLIC_OMENTUM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPECTRUM-OV-082_S1_INFRACOLIC_OMENTUM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPECTRUM-OV-083_S1_INFRACOLIC_OMENTUM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBS1 (Age)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBS5 (Age)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBS8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBS40 (Age)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBS9 (Pol η)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBS26 (MMRD1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBS44 (MMRD2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBS2 (APOBEC1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBS13 (APOBEC2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBS3 (HRD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S-Dup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M-Dup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L-Dup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S-Del</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L-Del</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clust-FBI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clust-SV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FBI/Inv</t>
   </si>
 </sst>
 </file>
@@ -1788,1359 +1840,2553 @@
       <c r="U1" t="s">
         <v>113</v>
       </c>
-      <c r="V1" t="s">
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
         <v>114</v>
       </c>
-      <c r="W1" t="s">
+      <c r="B2" t="n">
+        <v>0.0149084739951623</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.00111597500841346</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.00099381222222115</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.00123487978835402</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.000761555462756687</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.000614429960854269</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.00197454786387312</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.00111810189888181</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.0143769766125648</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.00116010024092001</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.00127166795458553</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.000645424552260446</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.000753713590291099</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.00178473961216233</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0.00441758741770144</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0.000805412173432799</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0.0191163749818189</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0.000567655063894545</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0.00119883892970905</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0.00621350315951579</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
         <v>115</v>
       </c>
+      <c r="B3" t="n">
+        <v>0.180300499046606</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.100494129605018</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.0759680912073891</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.0637614714325315</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.0764224688783064</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.0733608585767107</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.103144854926175</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.087579732472481</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.168470140984581</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.0844626843582001</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.0785901045123291</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.0594746803614286</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.0401788481655325</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.100987811961643</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0.121791064745622</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0.0743424782850497</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0.155819798019585</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0.0583446514820313</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0.110032148535585</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0.146974567174907</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.0893427212373494</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.198350735171886</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.231425051819974</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.169991075110417</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.212716673874906</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.226163325379812</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.169087850229969</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.205523953960583</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.0995011572202647</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.194398941000856</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.196733092881953</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.236983251394174</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.258440418775965</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.136434854859816</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.164171470060154</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.228598984391836</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.0918563875939661</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0.276222161968332</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0.137766992643442</v>
+      </c>
+      <c r="U4" t="n">
+        <v>0.124634068742511</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.206977459325866</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.114501533899324</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.14034622502327</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.129009170780171</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.112446364451616</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.120612851471069</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.0948768989325608</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.108718786959239</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.236125725487292</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.121029958067307</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.12484505464906</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.189078911033979</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.118880976240318</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.0957241461290508</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.158218726602913</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0.147222197117975</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0.234926086250237</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0.141340491496765</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0.0729446761399206</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0.156644831611819</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.122432746642936</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.0746824947996976</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.0876101341665427</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.111626564720361</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.0668489776933639</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.0944649125009858</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.0800377647905016</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.0835495975499603</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.0829297714958802</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.0834700797302454</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.0846045029052194</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.100840172955784</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.0463586034334431</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.105340747933134</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.083559237291145</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0.103344052017303</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0.102454311794786</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0.0643314873804924</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0.103196603274528</v>
+      </c>
+      <c r="U6" t="n">
+        <v>0.101301880534767</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.0758076935269384</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.0836493030202717</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.0839414203057991</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.104387087291043</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.0984312552616194</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.0750264662808179</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.103332483832364</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.102888027473815</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.0681836564476662</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.080076352604663</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.0808037040383064</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.0662714872569221</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.0927856698402666</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.116547474404358</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.0821325871350726</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0.0657254869198958</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0.0810173100732207</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0.0647093307453267</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0.135387316395743</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0.0909249476128633</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.142074582384371</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.0719128884118813</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.068947228161737</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.0894956944512929</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.0604453459276998</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.0649225403719104</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.100413943722652</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.0773905302595332</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.126004113717956</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.0753095430799633</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.0794780319322086</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.0485751224625608</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.0799565214218274</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0.0979638610221577</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0.115357606897879</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0.0801581552093951</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0.128616804691277</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0.0660336798403694</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0.0732242009450895</v>
+      </c>
+      <c r="U8" t="n">
+        <v>0.103956289496801</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.0695409527457119</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.0602604271235178</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.0589664001325093</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.173159572713011</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.0641805872519802</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.0536639704015834</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.0347887398554764</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.0481717530303242</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.10677508310425</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.0523757805915372</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.0747771411264382</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.0607786092764575</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.0677680190771766</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.0794576229407894</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0.0341610865391408</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0.0496675406002583</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0.077934273537893</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0.0541345198449363</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0.0452146084221344</v>
+      </c>
+      <c r="U9" t="n">
+        <v>0.0433527211411716</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.0287381392596309</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.087256536482439</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.0727252311115837</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.052607882143084</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.117839324507113</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.0740418767703255</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.0868309264604682</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.0832712106778489</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.030729442700315</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.107803231043926</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.0828300706957505</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.0905333405744002</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.115098393475093</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.105531485758645</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0.0697532239455372</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0.0631271490931954</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0.0457287210058605</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0.0680997822016543</v>
+      </c>
+      <c r="T10" t="n">
+        <v>0.120964056002321</v>
+      </c>
+      <c r="U10" t="n">
+        <v>0.0790906122236979</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>123</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.0698767318354275</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.207775976477551</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.179076405848974</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.104726601569733</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.189907446690638</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.217128768285931</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.22551198938596</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.201788305717334</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.0669039322292308</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.199913329282382</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.19606662930415</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.146819000132034</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.179778835980087</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.160227255378245</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0.166437409364835</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0.187008544191658</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0.0625299320513551</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0.206216239976197</v>
+      </c>
+      <c r="T11" t="n">
+        <v>0.200070558711527</v>
+      </c>
+      <c r="U11" t="n">
+        <v>0.146906578301945</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>124</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.00543231610400528</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.196838155894667</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.263059358421157</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.0256967872224841</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.00829188016560716</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.349511284441941</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.244366710576326</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.149292655616477</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.00362192468008515</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.0517943161258353</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.191702904353797</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.00849263667359963</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0.455122866728227</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0.0456928744763109</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0.275560511833</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0.266237334672358</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0.0137634899994981</v>
+      </c>
+      <c r="S12" t="n">
+        <v>0.0641723552015021</v>
+      </c>
+      <c r="T12" t="n">
+        <v>0.0049560559481992</v>
+      </c>
+      <c r="U12" t="n">
+        <v>0.00480264100282696</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>125</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.0370608066756776</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.313998610010341</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.217212383146714</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.108967170305679</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.0134353024166232</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.140571419223381</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.158247124053829</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.278606045678717</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.0188431962899998</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.172200791661818</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.177308820626793</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0.0154160932065718</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0.0586047355678503</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0.0319407969213477</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0.190263827394382</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0.0745150313890091</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0.0227148162517998</v>
+      </c>
+      <c r="S13" t="n">
+        <v>0.0465187701902108</v>
+      </c>
+      <c r="T13" t="n">
+        <v>0.00560223031265995</v>
+      </c>
+      <c r="U13" t="n">
+        <v>0.011713088114791</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>126</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0.211805009857887</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.0493651813134143</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.108332359458877</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.290737030912391</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.0267849546957611</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.0509210490949883</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.108830825669247</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.113087280557493</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.0435627955230203</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.182981654673743</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.121195658541388</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0.107570528982385</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0.0652604299633773</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0.0270852666590993</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0.0492902085002527</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0.0368520290372724</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0.0440933010585435</v>
+      </c>
+      <c r="S14" t="n">
+        <v>0.048910401401059</v>
+      </c>
+      <c r="T14" t="n">
+        <v>0.0100678733152868</v>
+      </c>
+      <c r="U14" t="n">
+        <v>0.102807690541369</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>127</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0.074519685570985</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.1670837745489</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.0862084013846566</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.199187592844044</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.300684446847988</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.192026892859069</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.118845379445731</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.180054183513412</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.066433137101507</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.354176607540573</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.0875115472452828</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0.197235419395536</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0.104011942220007</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0.440543870323423</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0.0905332791354257</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>0.247508716578371</v>
+      </c>
+      <c r="R15" t="n">
+        <v>0.0647331186919951</v>
+      </c>
+      <c r="S15" t="n">
+        <v>0.354385951523961</v>
+      </c>
+      <c r="T15" t="n">
+        <v>0.452934389204711</v>
+      </c>
+      <c r="U15" t="n">
+        <v>0.0666153485930557</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>128</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0.169351911102262</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.0362680296986978</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.0357461395247218</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.19509883765814</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.283257472680921</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.0485725976720374</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.0531435894023873</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.0759549671695571</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.125335959328878</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0.0412598457692637</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.0577418506540919</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0.302289026094491</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0.0286104697388909</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0.0782116863777572</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0.0516285691582016</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>0.0393117577749187</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0.133349954193854</v>
+      </c>
+      <c r="S16" t="n">
+        <v>0.0612388528217809</v>
+      </c>
+      <c r="T16" t="n">
+        <v>0.0442908867894752</v>
+      </c>
+      <c r="U16" t="n">
+        <v>0.0531081528346769</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>129</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0.00881594568895698</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.000462288121213516</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.0012772023970275</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.0161664203749406</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.0438871787477135</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.00193839165244923</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.00385212649595439</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.00190138070386371</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.0351000612937272</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.000973350517244337</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.0179880778036414</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0.0081064465773771</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0.00246178681217396</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0.00455288778427951</v>
+      </c>
+      <c r="P17" t="n">
+        <v>0.00391399335573105</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>0.000790558067720309</v>
+      </c>
+      <c r="R17" t="n">
+        <v>0.0789347864586685</v>
+      </c>
+      <c r="S17" t="n">
+        <v>0.0491929394594558</v>
+      </c>
+      <c r="T17" t="n">
+        <v>0.183302510306523</v>
+      </c>
+      <c r="U17" t="n">
+        <v>0.142990981562302</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>130</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0.00972542350892485</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.00037324393336548</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.00137668024881733</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.00239971304271593</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.054873569400561</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.00683928008969728</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.0461394471023763</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.0175826662341185</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.280792117269441</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.000530507872985546</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0.0272221937761137</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0.0616511580197588</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0.0279389358555744</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0.00306485890681048</v>
+      </c>
+      <c r="P18" t="n">
+        <v>0.00168107460776575</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>0.000795177118101918</v>
+      </c>
+      <c r="R18" t="n">
+        <v>0.265740961349732</v>
+      </c>
+      <c r="S18" t="n">
+        <v>0.00424453242290318</v>
+      </c>
+      <c r="T18" t="n">
+        <v>0.00803284414777309</v>
+      </c>
+      <c r="U18" t="n">
+        <v>0.191169073121764</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>131</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0.130063239378469</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.195349775695389</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.194493042296766</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.0821321304175874</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.15475333095812</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.14288765245671</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.130388241337161</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.130229655872387</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0.152796976461231</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0.106547235988051</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0.194016119615713</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0.109710067397624</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0.17997591657357</v>
+      </c>
+      <c r="O19" t="n">
+        <v>0.223003354974253</v>
+      </c>
+      <c r="P19" t="n">
+        <v>0.196060744114302</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>0.215965048438638</v>
+      </c>
+      <c r="R19" t="n">
+        <v>0.126110012262065</v>
+      </c>
+      <c r="S19" t="n">
+        <v>0.181527745552472</v>
+      </c>
+      <c r="T19" t="n">
+        <v>0.140132963490179</v>
+      </c>
+      <c r="U19" t="n">
+        <v>0.142462568410487</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>132</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0.353225662112833</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.0402609407840116</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.092294433121262</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.0796143172220169</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.114031864086706</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.0667314325097281</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.136186555916988</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.0532911646539748</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0.273513832052111</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0.0895356898504858</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0.125312827383179</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0.189528623652657</v>
+      </c>
+      <c r="N20" t="n">
+        <v>0.0780129165403299</v>
+      </c>
+      <c r="O20" t="n">
+        <v>0.14590440357672</v>
+      </c>
+      <c r="P20" t="n">
+        <v>0.14106779190094</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>0.11802434692361</v>
+      </c>
+      <c r="R20" t="n">
+        <v>0.250559559733844</v>
+      </c>
+      <c r="S20" t="n">
+        <v>0.189808451426655</v>
+      </c>
+      <c r="T20" t="n">
+        <v>0.150680246485193</v>
+      </c>
+      <c r="U20" t="n">
+        <v>0.284330455818727</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1" t="s">
+        <v>101</v>
+      </c>
+      <c r="J1" t="s">
+        <v>102</v>
+      </c>
+      <c r="K1" t="s">
+        <v>103</v>
+      </c>
+      <c r="L1" t="s">
+        <v>104</v>
+      </c>
+      <c r="M1" t="s">
+        <v>105</v>
+      </c>
+      <c r="N1" t="s">
+        <v>106</v>
+      </c>
+      <c r="O1" t="s">
+        <v>107</v>
+      </c>
+      <c r="P1" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>109</v>
+      </c>
+      <c r="R1" t="s">
+        <v>110</v>
+      </c>
+      <c r="S1" t="s">
+        <v>111</v>
+      </c>
+      <c r="T1" t="s">
+        <v>112</v>
+      </c>
+      <c r="U1" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>0.55867102797821</v>
+      <c r="A2" t="s">
+        <v>114</v>
       </c>
       <c r="B2" t="n">
         <v>0.653823517920692</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.337416099799313</v>
+        <v>-0.379195664522017</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.379195664522017</v>
+        <v>-0.388345311851232</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.388345311851232</v>
+        <v>-0.370290032650612</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.370290032650612</v>
+        <v>-0.405740686540713</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.405740686540713</v>
+        <v>-0.416759970706528</v>
       </c>
       <c r="H2" t="n">
-        <v>-0.416759970706528</v>
+        <v>-0.314890984850368</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.314890984850368</v>
+        <v>-0.379036366438699</v>
       </c>
       <c r="J2" t="n">
-        <v>-0.175396651095867</v>
+        <v>0.614015866517648</v>
       </c>
       <c r="K2" t="n">
-        <v>-0.379036366438699</v>
+        <v>-0.375890809350173</v>
       </c>
       <c r="L2" t="n">
-        <v>0.614015866517648</v>
+        <v>-0.367534703000738</v>
       </c>
       <c r="M2" t="n">
-        <v>-0.375890809350173</v>
+        <v>-0.414438563432522</v>
       </c>
       <c r="N2" t="n">
-        <v>-0.367534703000738</v>
+        <v>-0.406328020619258</v>
       </c>
       <c r="O2" t="n">
-        <v>-0.414438563432522</v>
+        <v>-0.329107086311861</v>
       </c>
       <c r="P2" t="n">
-        <v>-0.406328020619258</v>
+        <v>-0.131914228789296</v>
       </c>
       <c r="Q2" t="n">
-        <v>-0.329107086311861</v>
+        <v>-0.402455942894852</v>
       </c>
       <c r="R2" t="n">
-        <v>-0.131914228789296</v>
+        <v>0.968983406002764</v>
       </c>
       <c r="S2" t="n">
-        <v>-0.402455942894852</v>
+        <v>-0.420263278255262</v>
       </c>
       <c r="T2" t="n">
-        <v>0.968983406002764</v>
+        <v>-0.372989391074907</v>
       </c>
       <c r="U2" t="n">
-        <v>-0.420263278255262</v>
-      </c>
-      <c r="V2" t="n">
-        <v>-0.372989391074907</v>
-      </c>
-      <c r="W2" t="n">
         <v>0.00259478318362204</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>1.46191212775567</v>
+      <c r="A3" t="s">
+        <v>115</v>
       </c>
       <c r="B3" t="n">
         <v>1.6547219708436</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.220232635929218</v>
+        <v>-0.130100551073815</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.130100551073815</v>
+        <v>-0.678610977143744</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.678610977143744</v>
+        <v>-0.951604850227953</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.951604850227953</v>
+        <v>-0.668449087733363</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.668449087733363</v>
+        <v>-0.736920201729118</v>
       </c>
       <c r="H3" t="n">
-        <v>-0.736920201729118</v>
+        <v>-0.0708186380420548</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.0708186380420548</v>
+        <v>-0.418923448549546</v>
       </c>
       <c r="J3" t="n">
-        <v>0.806671746342279</v>
+        <v>1.39014296970378</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.418923448549546</v>
+        <v>-0.488634396625447</v>
       </c>
       <c r="L3" t="n">
-        <v>1.39014296970378</v>
+        <v>-0.619971191470381</v>
       </c>
       <c r="M3" t="n">
-        <v>-0.488634396625447</v>
+        <v>-1.04747641165838</v>
       </c>
       <c r="N3" t="n">
-        <v>-0.619971191470381</v>
+        <v>-1.47901635168261</v>
       </c>
       <c r="O3" t="n">
-        <v>-1.04747641165838</v>
+        <v>-0.119059635480957</v>
       </c>
       <c r="P3" t="n">
-        <v>-1.47901635168261</v>
+        <v>0.346192879547475</v>
       </c>
       <c r="Q3" t="n">
-        <v>-0.119059635480957</v>
+        <v>-0.714966854199836</v>
       </c>
       <c r="R3" t="n">
-        <v>0.346192879547475</v>
+        <v>1.10722548840639</v>
       </c>
       <c r="S3" t="n">
-        <v>-0.714966854199836</v>
+        <v>-1.07274884302543</v>
       </c>
       <c r="T3" t="n">
-        <v>1.10722548840639</v>
+        <v>0.0832116334155547</v>
       </c>
       <c r="U3" t="n">
-        <v>-1.07274884302543</v>
-      </c>
-      <c r="V3" t="n">
-        <v>0.0832116334155547</v>
-      </c>
-      <c r="W3" t="n">
         <v>0.909407102059476</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>-0.986761390406177</v>
+      <c r="A4" t="s">
+        <v>116</v>
       </c>
       <c r="B4" t="n">
         <v>-0.772044012093793</v>
       </c>
       <c r="C4" t="n">
-        <v>0.974089981270711</v>
+        <v>1.05135302009463</v>
       </c>
       <c r="D4" t="n">
-        <v>1.05135302009463</v>
+        <v>1.604593177777</v>
       </c>
       <c r="E4" t="n">
-        <v>1.604593177777</v>
+        <v>0.576975787416958</v>
       </c>
       <c r="F4" t="n">
-        <v>0.576975787416958</v>
+        <v>1.29165471031182</v>
       </c>
       <c r="G4" t="n">
-        <v>1.29165471031182</v>
+        <v>1.51657931504448</v>
       </c>
       <c r="H4" t="n">
-        <v>1.51657931504448</v>
+        <v>0.561867379264542</v>
       </c>
       <c r="I4" t="n">
-        <v>0.561867379264542</v>
+        <v>1.1713407657516</v>
       </c>
       <c r="J4" t="n">
-        <v>-0.0814312049293967</v>
+        <v>-0.602121991185793</v>
       </c>
       <c r="K4" t="n">
-        <v>1.1713407657516</v>
+        <v>0.985250634561736</v>
       </c>
       <c r="L4" t="n">
-        <v>-0.602121991185793</v>
+        <v>1.02429442096836</v>
       </c>
       <c r="M4" t="n">
-        <v>0.985250634561736</v>
+        <v>1.69756620097136</v>
       </c>
       <c r="N4" t="n">
-        <v>1.02429442096836</v>
+        <v>2.05648417324653</v>
       </c>
       <c r="O4" t="n">
-        <v>1.69756620097136</v>
+        <v>0.0156747398338641</v>
       </c>
       <c r="P4" t="n">
-        <v>2.05648417324653</v>
+        <v>0.479630186904212</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.0156747398338641</v>
+        <v>1.55732102983817</v>
       </c>
       <c r="R4" t="n">
-        <v>0.479630186904212</v>
+        <v>-0.729997454146968</v>
       </c>
       <c r="S4" t="n">
-        <v>1.55732102983817</v>
+        <v>2.35392265133467</v>
       </c>
       <c r="T4" t="n">
-        <v>-0.729997454146968</v>
+        <v>0.0379576527450984</v>
       </c>
       <c r="U4" t="n">
-        <v>2.35392265133467</v>
-      </c>
-      <c r="V4" t="n">
-        <v>0.0379576527450984</v>
-      </c>
-      <c r="W4" t="n">
         <v>-0.181719172844014</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>0.135688031108185</v>
+      <c r="A5" t="s">
+        <v>117</v>
       </c>
       <c r="B5" t="n">
         <v>1.49450464223431</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0976357568493115</v>
+        <v>-0.188137301189861</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.188137301189861</v>
+        <v>0.282118725980557</v>
       </c>
       <c r="E5" t="n">
-        <v>0.282118725980557</v>
+        <v>0.0758358161710585</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0758358161710585</v>
+        <v>-0.225532053365704</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.225532053365704</v>
+        <v>-0.0769390706409609</v>
       </c>
       <c r="H5" t="n">
-        <v>-0.0769390706409609</v>
+        <v>-0.545216549298544</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.545216549298544</v>
+        <v>-0.29335703816155</v>
       </c>
       <c r="J5" t="n">
-        <v>0.414723455386916</v>
+        <v>2.02487073476144</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.29335703816155</v>
+        <v>-0.0693496245178621</v>
       </c>
       <c r="L5" t="n">
-        <v>2.02487073476144</v>
+        <v>0.0000678103124660837</v>
       </c>
       <c r="M5" t="n">
-        <v>-0.0693496245178621</v>
+        <v>1.16883233408038</v>
       </c>
       <c r="N5" t="n">
-        <v>0.0000678103124660837</v>
+        <v>-0.108451336028929</v>
       </c>
       <c r="O5" t="n">
-        <v>1.16883233408038</v>
+        <v>-0.529800497361924</v>
       </c>
       <c r="P5" t="n">
-        <v>-0.108451336028929</v>
+        <v>0.607317102240238</v>
       </c>
       <c r="Q5" t="n">
-        <v>-0.529800497361924</v>
+        <v>0.407230196830939</v>
       </c>
       <c r="R5" t="n">
-        <v>0.607317102240238</v>
+        <v>2.00304274776986</v>
       </c>
       <c r="S5" t="n">
-        <v>0.407230196830939</v>
+        <v>0.300209861197939</v>
       </c>
       <c r="T5" t="n">
-        <v>2.00304274776986</v>
+        <v>-0.944283417926256</v>
       </c>
       <c r="U5" t="n">
-        <v>0.300209861197939</v>
-      </c>
-      <c r="V5" t="n">
-        <v>-0.944283417926256</v>
-      </c>
-      <c r="W5" t="n">
         <v>0.57867935988357</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>0.0770539733447342</v>
+      <c r="A6" t="s">
+        <v>118</v>
       </c>
       <c r="B6" t="n">
         <v>0.302866400919668</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.543608283194567</v>
+        <v>-0.622092390422354</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.622092390422354</v>
+        <v>-0.371674157594627</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.371674157594627</v>
+        <v>0.0935424165574429</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0935424165574429</v>
+        <v>-0.773833590414737</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.773833590414737</v>
+        <v>-0.238891873975283</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.238891873975283</v>
+        <v>-0.518356726906565</v>
       </c>
       <c r="I6" t="n">
-        <v>-0.518356726906565</v>
+        <v>-0.450329848320705</v>
       </c>
       <c r="J6" t="n">
-        <v>0.965469451024862</v>
+        <v>-0.462336351651963</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.450329848320705</v>
+        <v>-0.451870169126869</v>
       </c>
       <c r="L6" t="n">
-        <v>-0.462336351651963</v>
+        <v>-0.429895527145101</v>
       </c>
       <c r="M6" t="n">
-        <v>-0.451870169126869</v>
+        <v>-0.115398217352912</v>
       </c>
       <c r="N6" t="n">
-        <v>-0.429895527145101</v>
+        <v>-1.17074776527235</v>
       </c>
       <c r="O6" t="n">
-        <v>-0.115398217352912</v>
+        <v>-0.0282186480166078</v>
       </c>
       <c r="P6" t="n">
-        <v>-1.17074776527235</v>
+        <v>-0.450143119182933</v>
       </c>
       <c r="Q6" t="n">
-        <v>-0.0282186480166078</v>
+        <v>-0.0668961705362156</v>
       </c>
       <c r="R6" t="n">
-        <v>-0.450143119182933</v>
+        <v>-0.0841311171398445</v>
       </c>
       <c r="S6" t="n">
-        <v>-0.0668961705362156</v>
+        <v>-0.822599297549716</v>
       </c>
       <c r="T6" t="n">
-        <v>-0.0841311171398445</v>
+        <v>-0.0697523651244699</v>
       </c>
       <c r="U6" t="n">
-        <v>-0.822599297549716</v>
-      </c>
-      <c r="V6" t="n">
-        <v>-0.0697523651244699</v>
-      </c>
-      <c r="W6" t="n">
         <v>-0.106454589461453</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>0.0404947882781174</v>
+      <c r="A7" t="s">
+        <v>119</v>
       </c>
       <c r="B7" t="n">
         <v>-0.414864946813832</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.550029577940684</v>
+        <v>-0.202125390528597</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.202125390528597</v>
+        <v>-0.19420037184982</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.19420037184982</v>
+        <v>0.360481945102388</v>
       </c>
       <c r="F7" t="n">
-        <v>0.360481945102388</v>
+        <v>0.198902735588543</v>
       </c>
       <c r="G7" t="n">
-        <v>0.198902735588543</v>
+        <v>-0.436059312312254</v>
       </c>
       <c r="H7" t="n">
-        <v>-0.436059312312254</v>
+        <v>0.33187099832582</v>
       </c>
       <c r="I7" t="n">
-        <v>0.33187099832582</v>
+        <v>0.319813084885189</v>
       </c>
       <c r="J7" t="n">
-        <v>-0.0276786452588162</v>
+        <v>-0.621701855324189</v>
       </c>
       <c r="K7" t="n">
-        <v>0.319813084885189</v>
+        <v>-0.299058027469004</v>
       </c>
       <c r="L7" t="n">
-        <v>-0.621701855324189</v>
+        <v>-0.27932529002674</v>
       </c>
       <c r="M7" t="n">
-        <v>-0.299058027469004</v>
+        <v>-0.673578198506931</v>
       </c>
       <c r="N7" t="n">
-        <v>-0.27932529002674</v>
+        <v>0.0457403856232626</v>
       </c>
       <c r="O7" t="n">
-        <v>-0.673578198506931</v>
+        <v>0.690388115633142</v>
       </c>
       <c r="P7" t="n">
-        <v>0.0457403856232626</v>
+        <v>-0.24327325241873</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.690388115633142</v>
+        <v>-0.688390957230675</v>
       </c>
       <c r="R7" t="n">
-        <v>-0.24327325241873</v>
+        <v>-0.27353024844425</v>
       </c>
       <c r="S7" t="n">
-        <v>-0.688390957230675</v>
+        <v>-0.715958845414613</v>
       </c>
       <c r="T7" t="n">
-        <v>-0.27353024844425</v>
+        <v>1.20150507818257</v>
       </c>
       <c r="U7" t="n">
-        <v>-0.715958845414613</v>
-      </c>
-      <c r="V7" t="n">
-        <v>1.20150507818257</v>
-      </c>
-      <c r="W7" t="n">
         <v>-0.00474022315537953</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>0.233917569677791</v>
+      <c r="A8" t="s">
+        <v>120</v>
       </c>
       <c r="B8" t="n">
         <v>0.515471420320347</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0175194910141728</v>
+        <v>-0.349484440304065</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.349484440304065</v>
+        <v>-0.386045205427395</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.386045205427395</v>
+        <v>-0.132722981608746</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.132722981608746</v>
+        <v>-0.490856712224145</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.490856712224145</v>
+        <v>-0.435661699754898</v>
       </c>
       <c r="H8" t="n">
-        <v>-0.435661699754898</v>
+        <v>0.00187758403215112</v>
       </c>
       <c r="I8" t="n">
-        <v>0.00187758403215112</v>
+        <v>-0.281955876635323</v>
       </c>
       <c r="J8" t="n">
-        <v>-0.317804427028122</v>
+        <v>0.317354110589388</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.281955876635323</v>
+        <v>-0.307610360655606</v>
       </c>
       <c r="L8" t="n">
-        <v>0.317354110589388</v>
+        <v>-0.256221081712159</v>
       </c>
       <c r="M8" t="n">
-        <v>-0.307610360655606</v>
+        <v>-0.637193249610474</v>
       </c>
       <c r="N8" t="n">
-        <v>-0.256221081712159</v>
+        <v>-0.250322246252809</v>
       </c>
       <c r="O8" t="n">
-        <v>-0.637193249610474</v>
+        <v>-0.0283271227076605</v>
       </c>
       <c r="P8" t="n">
-        <v>-0.250322246252809</v>
+        <v>0.186103595560284</v>
       </c>
       <c r="Q8" t="n">
-        <v>-0.0283271227076605</v>
+        <v>-0.247836497742732</v>
       </c>
       <c r="R8" t="n">
-        <v>0.186103595560284</v>
+        <v>0.349563457904469</v>
       </c>
       <c r="S8" t="n">
-        <v>-0.247836497742732</v>
+        <v>-0.421963532837897</v>
       </c>
       <c r="T8" t="n">
-        <v>0.349563457904469</v>
+        <v>-0.333318532719887</v>
       </c>
       <c r="U8" t="n">
-        <v>-0.421963532837897</v>
-      </c>
-      <c r="V8" t="n">
-        <v>-0.333318532719887</v>
-      </c>
-      <c r="W8" t="n">
         <v>0.0455477488219248</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>-0.465745865029967</v>
+      <c r="A9" t="s">
+        <v>121</v>
       </c>
       <c r="B9" t="n">
         <v>-0.2499908690813</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.523146901586802</v>
+        <v>-0.382605772579067</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.382605772579067</v>
+        <v>-0.401096887363094</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.401096887363094</v>
+        <v>1.23067669727648</v>
       </c>
       <c r="F9" t="n">
-        <v>1.23067669727648</v>
+        <v>-0.326588292719027</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.326588292719027</v>
+        <v>-0.476866432720395</v>
       </c>
       <c r="H9" t="n">
-        <v>-0.476866432720395</v>
+        <v>-0.746585733035012</v>
       </c>
       <c r="I9" t="n">
-        <v>-0.746585733035012</v>
+        <v>-0.555347965591385</v>
       </c>
       <c r="J9" t="n">
-        <v>-0.604990942230045</v>
+        <v>0.28206957720551</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.555347965591385</v>
+        <v>-0.495274136583367</v>
       </c>
       <c r="L9" t="n">
-        <v>0.28206957720551</v>
+        <v>-0.175167885440641</v>
       </c>
       <c r="M9" t="n">
-        <v>-0.495274136583367</v>
+        <v>-0.375201162214969</v>
       </c>
       <c r="N9" t="n">
-        <v>-0.175167885440641</v>
+        <v>-0.27532536379984</v>
       </c>
       <c r="O9" t="n">
-        <v>-0.375201162214969</v>
+        <v>-0.108285720636435</v>
       </c>
       <c r="P9" t="n">
-        <v>-0.27532536379984</v>
+        <v>-0.755554641409861</v>
       </c>
       <c r="Q9" t="n">
-        <v>-0.108285720636435</v>
+        <v>-0.533973774913479</v>
       </c>
       <c r="R9" t="n">
-        <v>-0.755554641409861</v>
+        <v>-0.130053758599217</v>
       </c>
       <c r="S9" t="n">
-        <v>-0.533973774913479</v>
+        <v>-0.470142474233395</v>
       </c>
       <c r="T9" t="n">
-        <v>-0.130053758599217</v>
+        <v>-0.59760434877578</v>
       </c>
       <c r="U9" t="n">
-        <v>-0.470142474233395</v>
-      </c>
-      <c r="V9" t="n">
-        <v>-0.59760434877578</v>
-      </c>
-      <c r="W9" t="n">
         <v>-0.62420995411974</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>0.345911669571026</v>
+      <c r="A10" t="s">
+        <v>122</v>
       </c>
       <c r="B10" t="n">
         <v>-1.03329301267967</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.405759961565337</v>
+        <v>-0.186141639941228</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.186141639941228</v>
+        <v>-0.396506514524694</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.396506514524694</v>
+        <v>-0.68773868429233</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.68773868429233</v>
+        <v>0.256595210123654</v>
       </c>
       <c r="G10" t="n">
-        <v>0.256595210123654</v>
+        <v>-0.377445873253773</v>
       </c>
       <c r="H10" t="n">
-        <v>-0.377445873253773</v>
+        <v>-0.19230305466677</v>
       </c>
       <c r="I10" t="n">
-        <v>-0.19230305466677</v>
+        <v>-0.243835876051517</v>
       </c>
       <c r="J10" t="n">
-        <v>-0.388814598292494</v>
+        <v>-1.00446557509809</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.243835876051517</v>
+        <v>0.111306023171069</v>
       </c>
       <c r="L10" t="n">
-        <v>-1.00446557509809</v>
+        <v>-0.250222112844393</v>
       </c>
       <c r="M10" t="n">
-        <v>0.111306023171069</v>
+        <v>-0.138704437002629</v>
       </c>
       <c r="N10" t="n">
-        <v>-0.250222112844393</v>
+        <v>0.216915663236609</v>
       </c>
       <c r="O10" t="n">
-        <v>-0.138704437002629</v>
+        <v>0.0784187222832774</v>
       </c>
       <c r="P10" t="n">
-        <v>0.216915663236609</v>
+        <v>-0.439531273745602</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.0784187222832774</v>
+        <v>-0.535454755478304</v>
       </c>
       <c r="R10" t="n">
-        <v>-0.439531273745602</v>
+        <v>-0.787326011992009</v>
       </c>
       <c r="S10" t="n">
-        <v>-0.535454755478304</v>
+        <v>-0.463467599919065</v>
       </c>
       <c r="T10" t="n">
-        <v>-0.787326011992009</v>
+        <v>0.30183090866006</v>
       </c>
       <c r="U10" t="n">
-        <v>-0.463467599919065</v>
-      </c>
-      <c r="V10" t="n">
-        <v>0.30183090866006</v>
-      </c>
-      <c r="W10" t="n">
         <v>-0.30435700935969</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>-0.593846267368161</v>
+      <c r="A11" t="s">
+        <v>123</v>
       </c>
       <c r="B11" t="n">
         <v>-1.15414279081911</v>
       </c>
       <c r="C11" t="n">
-        <v>0.998990577241354</v>
+        <v>1.05681282892511</v>
       </c>
       <c r="D11" t="n">
-        <v>1.05681282892511</v>
+        <v>0.596669068673392</v>
       </c>
       <c r="E11" t="n">
-        <v>0.596669068673392</v>
+        <v>-0.595390525450417</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.595390525450417</v>
+        <v>0.7703244841088</v>
       </c>
       <c r="G11" t="n">
-        <v>0.7703244841088</v>
+        <v>1.20676729504782</v>
       </c>
       <c r="H11" t="n">
-        <v>1.20676729504782</v>
+        <v>1.34117651426268</v>
       </c>
       <c r="I11" t="n">
-        <v>1.34117651426268</v>
+        <v>0.960811764156139</v>
       </c>
       <c r="J11" t="n">
-        <v>-0.0881588100492298</v>
+        <v>-1.20180605404257</v>
       </c>
       <c r="K11" t="n">
-        <v>0.960811764156139</v>
+        <v>0.930750035417141</v>
       </c>
       <c r="L11" t="n">
-        <v>-1.20180605404257</v>
+        <v>0.869075419603146</v>
       </c>
       <c r="M11" t="n">
-        <v>0.930750035417141</v>
+        <v>0.0794820990614283</v>
       </c>
       <c r="N11" t="n">
-        <v>0.869075419603146</v>
+        <v>0.60793121771483</v>
       </c>
       <c r="O11" t="n">
-        <v>0.0794820990614283</v>
+        <v>0.294458311327927</v>
       </c>
       <c r="P11" t="n">
-        <v>0.60793121771483</v>
+        <v>0.39402647714176</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.294458311327927</v>
+        <v>0.723846022331551</v>
       </c>
       <c r="R11" t="n">
-        <v>0.39402647714176</v>
+        <v>-1.27193493907841</v>
       </c>
       <c r="S11" t="n">
-        <v>0.723846022331551</v>
+        <v>1.03180538097325</v>
       </c>
       <c r="T11" t="n">
-        <v>-1.27193493907841</v>
+        <v>0.933270914272267</v>
       </c>
       <c r="U11" t="n">
-        <v>1.03180538097325</v>
-      </c>
-      <c r="V11" t="n">
-        <v>0.933270914272267</v>
-      </c>
-      <c r="W11" t="n">
         <v>0.0808862506754261</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>-0.753265289843352</v>
+      <c r="A12" t="s">
+        <v>124</v>
       </c>
       <c r="B12" t="n">
         <v>-0.791588888631569</v>
       </c>
       <c r="C12" t="n">
-        <v>0.957609756671358</v>
+        <v>0.437698364532612</v>
       </c>
       <c r="D12" t="n">
-        <v>0.437698364532612</v>
+        <v>0.862998241715303</v>
       </c>
       <c r="E12" t="n">
-        <v>0.862998241715303</v>
+        <v>-0.661442096531054</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.661442096531054</v>
+        <v>-0.773223588730698</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.773223588730698</v>
+        <v>1.41822816983595</v>
       </c>
       <c r="H12" t="n">
-        <v>1.41822816983595</v>
+        <v>0.742946347015174</v>
       </c>
       <c r="I12" t="n">
-        <v>0.742946347015174</v>
+        <v>0.1323415504395</v>
       </c>
       <c r="J12" t="n">
-        <v>-0.752222956623928</v>
+        <v>-0.803215969096286</v>
       </c>
       <c r="K12" t="n">
-        <v>0.1323415504395</v>
+        <v>-0.493833001348481</v>
       </c>
       <c r="L12" t="n">
-        <v>-0.803215969096286</v>
+        <v>0.404717660976818</v>
       </c>
       <c r="M12" t="n">
-        <v>-0.493833001348481</v>
+        <v>-0.77193424762943</v>
       </c>
       <c r="N12" t="n">
-        <v>0.404717660976818</v>
+        <v>2.09650931336335</v>
       </c>
       <c r="O12" t="n">
-        <v>-0.77193424762943</v>
+        <v>-0.533018976310836</v>
       </c>
       <c r="P12" t="n">
-        <v>2.09650931336335</v>
+        <v>0.943285805333189</v>
       </c>
       <c r="Q12" t="n">
-        <v>-0.533018976310836</v>
+        <v>0.88340851603469</v>
       </c>
       <c r="R12" t="n">
-        <v>0.943285805333189</v>
+        <v>-0.738082653477906</v>
       </c>
       <c r="S12" t="n">
-        <v>0.88340851603469</v>
+        <v>-0.414336128779038</v>
       </c>
       <c r="T12" t="n">
-        <v>-0.738082653477906</v>
+        <v>-0.794647627797327</v>
       </c>
       <c r="U12" t="n">
-        <v>-0.414336128779038</v>
-      </c>
-      <c r="V12" t="n">
-        <v>-0.794647627797327</v>
-      </c>
-      <c r="W12" t="n">
         <v>-0.79563292185626</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
-        <v>-0.575551396360498</v>
+      <c r="A13" t="s">
+        <v>125</v>
       </c>
       <c r="B13" t="n">
         <v>-0.646793349048476</v>
       </c>
       <c r="C13" t="n">
-        <v>0.507786831736535</v>
+        <v>2.33472417593212</v>
       </c>
       <c r="D13" t="n">
-        <v>2.33472417593212</v>
+        <v>1.29272186315313</v>
       </c>
       <c r="E13" t="n">
-        <v>1.29272186315313</v>
+        <v>0.127351894897867</v>
       </c>
       <c r="F13" t="n">
-        <v>0.127351894897867</v>
+        <v>-0.901145965905741</v>
       </c>
       <c r="G13" t="n">
-        <v>-0.901145965905741</v>
+        <v>0.467603824671809</v>
       </c>
       <c r="H13" t="n">
-        <v>0.467603824671809</v>
+        <v>0.657900790574586</v>
       </c>
       <c r="I13" t="n">
-        <v>0.657900790574586</v>
+        <v>1.95368717217853</v>
       </c>
       <c r="J13" t="n">
-        <v>0.0032767656540103</v>
+        <v>-0.842924480205492</v>
       </c>
       <c r="K13" t="n">
-        <v>1.95368717217853</v>
+        <v>0.808126234735768</v>
       </c>
       <c r="L13" t="n">
-        <v>-0.842924480205492</v>
+        <v>0.863119369272829</v>
       </c>
       <c r="M13" t="n">
-        <v>0.808126234735768</v>
+        <v>-0.879820735538346</v>
       </c>
       <c r="N13" t="n">
-        <v>0.863119369272829</v>
+        <v>-0.414851011182359</v>
       </c>
       <c r="O13" t="n">
-        <v>-0.879820735538346</v>
+        <v>-0.70191546898585</v>
       </c>
       <c r="P13" t="n">
-        <v>-0.414851011182359</v>
+        <v>1.00259321231163</v>
       </c>
       <c r="Q13" t="n">
-        <v>-0.70191546898585</v>
+        <v>-0.24356047140334</v>
       </c>
       <c r="R13" t="n">
-        <v>1.00259321231163</v>
+        <v>-0.801242547918978</v>
       </c>
       <c r="S13" t="n">
-        <v>-0.24356047140334</v>
+        <v>-0.544968738505398</v>
       </c>
       <c r="T13" t="n">
-        <v>-0.801242547918978</v>
+        <v>-0.985476965398001</v>
       </c>
       <c r="U13" t="n">
-        <v>-0.544968738505398</v>
-      </c>
-      <c r="V13" t="n">
-        <v>-0.985476965398001</v>
-      </c>
-      <c r="W13" t="n">
         <v>-0.919687357008204</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
-        <v>-0.205734423789736</v>
+      <c r="A14" t="s">
+        <v>126</v>
       </c>
       <c r="B14" t="n">
         <v>0.870982793371001</v>
       </c>
       <c r="C14" t="n">
-        <v>0.129596335797766</v>
+        <v>-0.530890946522053</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.530890946522053</v>
+        <v>-0.0219976578598537</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.0219976578598537</v>
+        <v>1.55217489105105</v>
       </c>
       <c r="F14" t="n">
-        <v>1.55217489105105</v>
+        <v>-0.725760807071407</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.725760807071407</v>
+        <v>-0.51746363497366</v>
       </c>
       <c r="H14" t="n">
-        <v>-0.51746363497366</v>
+        <v>-0.0176958391691852</v>
       </c>
       <c r="I14" t="n">
-        <v>-0.0176958391691852</v>
+        <v>0.0190378386876468</v>
       </c>
       <c r="J14" t="n">
-        <v>1.13280383417234</v>
+        <v>-0.580966179555527</v>
       </c>
       <c r="K14" t="n">
-        <v>0.0190378386876468</v>
+        <v>0.622234040738586</v>
       </c>
       <c r="L14" t="n">
-        <v>-0.580966179555527</v>
+        <v>0.0890140401562253</v>
       </c>
       <c r="M14" t="n">
-        <v>0.622234040738586</v>
+        <v>-0.0285723393823273</v>
       </c>
       <c r="N14" t="n">
-        <v>0.0890140401562253</v>
+        <v>-0.393713187402756</v>
       </c>
       <c r="O14" t="n">
-        <v>-0.0285723393823273</v>
+        <v>-0.723169081514</v>
       </c>
       <c r="P14" t="n">
-        <v>-0.393713187402756</v>
+        <v>-0.531537970216421</v>
       </c>
       <c r="Q14" t="n">
-        <v>-0.723169081514</v>
+        <v>-0.638880838757158</v>
       </c>
       <c r="R14" t="n">
-        <v>-0.531537970216421</v>
+        <v>-0.576387857934643</v>
       </c>
       <c r="S14" t="n">
-        <v>-0.638880838757158</v>
+        <v>-0.534815747614707</v>
       </c>
       <c r="T14" t="n">
-        <v>-0.576387857934643</v>
+        <v>-0.870031073821448</v>
       </c>
       <c r="U14" t="n">
-        <v>-0.534815747614707</v>
-      </c>
-      <c r="V14" t="n">
-        <v>-0.870031073821448</v>
-      </c>
-      <c r="W14" t="n">
         <v>-0.0696761634730108</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
-        <v>-0.0444900805219199</v>
+      <c r="A15" t="s">
+        <v>127</v>
       </c>
       <c r="B15" t="n">
         <v>-0.626580324170176</v>
       </c>
       <c r="C15" t="n">
-        <v>0.139015530391162</v>
+        <v>0.122368608608379</v>
       </c>
       <c r="D15" t="n">
-        <v>0.122368608608379</v>
+        <v>-0.532005296955358</v>
       </c>
       <c r="E15" t="n">
-        <v>-0.532005296955358</v>
+        <v>0.382125072651379</v>
       </c>
       <c r="F15" t="n">
-        <v>0.382125072651379</v>
+        <v>1.20335025107636</v>
       </c>
       <c r="G15" t="n">
-        <v>1.20335025107636</v>
+        <v>0.324186851998935</v>
       </c>
       <c r="H15" t="n">
-        <v>0.324186851998935</v>
+        <v>-0.2679349630077</v>
       </c>
       <c r="I15" t="n">
-        <v>-0.2679349630077</v>
+        <v>0.227313993572846</v>
       </c>
       <c r="J15" t="n">
-        <v>-0.742637008541527</v>
+        <v>-0.692009713828217</v>
       </c>
       <c r="K15" t="n">
-        <v>0.227313993572846</v>
+        <v>1.63616277162404</v>
       </c>
       <c r="L15" t="n">
-        <v>-0.692009713828217</v>
+        <v>-0.521461362343701</v>
       </c>
       <c r="M15" t="n">
-        <v>1.63616277162404</v>
+        <v>0.366329765453922</v>
       </c>
       <c r="N15" t="n">
-        <v>-0.521461362343701</v>
+        <v>-0.387954369046413</v>
       </c>
       <c r="O15" t="n">
-        <v>0.366329765453922</v>
+        <v>2.33497232079654</v>
       </c>
       <c r="P15" t="n">
-        <v>-0.387954369046413</v>
+        <v>-0.497012108866951</v>
       </c>
       <c r="Q15" t="n">
-        <v>2.33497232079654</v>
+        <v>0.773098013141497</v>
       </c>
       <c r="R15" t="n">
-        <v>-0.497012108866951</v>
+        <v>-0.705764799494448</v>
       </c>
       <c r="S15" t="n">
-        <v>0.773098013141497</v>
+        <v>1.63785660294322</v>
       </c>
       <c r="T15" t="n">
-        <v>-0.705764799494448</v>
+        <v>2.43522573435228</v>
       </c>
       <c r="U15" t="n">
-        <v>1.63785660294322</v>
-      </c>
-      <c r="V15" t="n">
-        <v>2.43522573435228</v>
-      </c>
-      <c r="W15" t="n">
         <v>-0.690535415278506</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="n">
-        <v>0.0894019623800398</v>
+      <c r="A16" t="s">
+        <v>128</v>
       </c>
       <c r="B16" t="n">
         <v>0.90187406248223</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.802758891834407</v>
+        <v>-0.675112897339848</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.675112897339848</v>
+        <v>-0.681297072238712</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.681297072238712</v>
+        <v>1.20696410799265</v>
       </c>
       <c r="F16" t="n">
-        <v>1.20696410799265</v>
+        <v>2.25160615149497</v>
       </c>
       <c r="G16" t="n">
-        <v>2.25160615149497</v>
+        <v>-0.529309040136736</v>
       </c>
       <c r="H16" t="n">
-        <v>-0.529309040136736</v>
+        <v>-0.475144747089425</v>
       </c>
       <c r="I16" t="n">
-        <v>-0.475144747089425</v>
+        <v>-0.204839696657985</v>
       </c>
       <c r="J16" t="n">
-        <v>0.707131298751438</v>
+        <v>0.38030389757025</v>
       </c>
       <c r="K16" t="n">
-        <v>-0.204839696657985</v>
+        <v>-0.615962016210663</v>
       </c>
       <c r="L16" t="n">
-        <v>0.38030389757025</v>
+        <v>-0.420657321900764</v>
       </c>
       <c r="M16" t="n">
-        <v>-0.615962016210663</v>
+        <v>2.47712190322863</v>
       </c>
       <c r="N16" t="n">
-        <v>-0.420657321900764</v>
+        <v>-0.765851701117687</v>
       </c>
       <c r="O16" t="n">
-        <v>2.47712190322863</v>
+        <v>-0.178098541186874</v>
       </c>
       <c r="P16" t="n">
-        <v>-0.765851701117687</v>
+        <v>-0.493097087701602</v>
       </c>
       <c r="Q16" t="n">
-        <v>-0.178098541186874</v>
+        <v>-0.63904602406547</v>
       </c>
       <c r="R16" t="n">
-        <v>-0.493097087701602</v>
+        <v>0.475266302219576</v>
       </c>
       <c r="S16" t="n">
-        <v>-0.63904602406547</v>
+        <v>-0.379219344898934</v>
       </c>
       <c r="T16" t="n">
-        <v>0.475266302219576</v>
+        <v>-0.580045479112795</v>
       </c>
       <c r="U16" t="n">
-        <v>-0.379219344898934</v>
-      </c>
-      <c r="V16" t="n">
-        <v>-0.580045479112795</v>
-      </c>
-      <c r="W16" t="n">
         <v>-0.475564655229996</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="n">
-        <v>-0.129137395127345</v>
+      <c r="A17" t="s">
+        <v>129</v>
       </c>
       <c r="B17" t="n">
         <v>-0.245281255939389</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.319456439820845</v>
+        <v>-0.321374071106152</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.321374071106152</v>
+        <v>-0.313951080534249</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.313951080534249</v>
+        <v>-0.178326355390406</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.178326355390406</v>
+        <v>0.0741798703001086</v>
       </c>
       <c r="G17" t="n">
-        <v>0.0741798703001086</v>
+        <v>-0.307928359181948</v>
       </c>
       <c r="H17" t="n">
-        <v>-0.307928359181948</v>
+        <v>-0.290496297771228</v>
       </c>
       <c r="I17" t="n">
-        <v>-0.290496297771228</v>
+        <v>-0.308265489025616</v>
       </c>
       <c r="J17" t="n">
-        <v>0.326334467880177</v>
+        <v>-0.00586129715888197</v>
       </c>
       <c r="K17" t="n">
-        <v>-0.308265489025616</v>
+        <v>-0.316718843605564</v>
       </c>
       <c r="L17" t="n">
-        <v>-0.00586129715888197</v>
+        <v>-0.161733019968742</v>
       </c>
       <c r="M17" t="n">
-        <v>-0.316718843605564</v>
+        <v>-0.251744028003077</v>
       </c>
       <c r="N17" t="n">
-        <v>-0.161733019968742</v>
+        <v>-0.303160793498876</v>
       </c>
       <c r="O17" t="n">
-        <v>-0.251744028003077</v>
+        <v>-0.284113117857983</v>
       </c>
       <c r="P17" t="n">
-        <v>-0.303160793498876</v>
+        <v>-0.289932757371378</v>
       </c>
       <c r="Q17" t="n">
-        <v>-0.284113117857983</v>
+        <v>-0.318383885769756</v>
       </c>
       <c r="R17" t="n">
-        <v>-0.289932757371378</v>
+        <v>0.393425795089351</v>
       </c>
       <c r="S17" t="n">
-        <v>-0.318383885769756</v>
+        <v>0.122509630753378</v>
       </c>
       <c r="T17" t="n">
-        <v>0.393425795089351</v>
+        <v>1.34410325053068</v>
       </c>
       <c r="U17" t="n">
-        <v>0.122509630753378</v>
-      </c>
-      <c r="V17" t="n">
-        <v>1.34410325053068</v>
-      </c>
-      <c r="W17" t="n">
         <v>0.976908679655748</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="n">
-        <v>-0.461719464901485</v>
+      <c r="A18" t="s">
+        <v>130</v>
       </c>
       <c r="B18" t="n">
         <v>-0.443212011398654</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.52577700593981</v>
+        <v>-0.525908312086709</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.525908312086709</v>
+        <v>-0.517035463720882</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.517035463720882</v>
+        <v>-0.507989334221928</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.507989334221928</v>
+        <v>-0.0439912075210081</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.0439912075210081</v>
+        <v>-0.468732627432272</v>
       </c>
       <c r="H18" t="n">
-        <v>-0.468732627432272</v>
+        <v>-0.121222359679859</v>
       </c>
       <c r="I18" t="n">
-        <v>-0.121222359679859</v>
+        <v>-0.373734634308963</v>
       </c>
       <c r="J18" t="n">
-        <v>0.242200241791388</v>
+        <v>1.95368516456214</v>
       </c>
       <c r="K18" t="n">
-        <v>-0.373734634308963</v>
+        <v>-0.524517711539196</v>
       </c>
       <c r="L18" t="n">
-        <v>1.95368516456214</v>
+        <v>-0.288497469895774</v>
       </c>
       <c r="M18" t="n">
-        <v>-0.524517711539196</v>
+        <v>0.0159393682196303</v>
       </c>
       <c r="N18" t="n">
-        <v>-0.288497469895774</v>
+        <v>-0.282159704667895</v>
       </c>
       <c r="O18" t="n">
-        <v>0.0159393682196303</v>
+        <v>-0.502107806612864</v>
       </c>
       <c r="P18" t="n">
-        <v>-0.282159704667895</v>
+        <v>-0.514343867902819</v>
       </c>
       <c r="Q18" t="n">
-        <v>-0.502107806612864</v>
+        <v>-0.52217738356536</v>
       </c>
       <c r="R18" t="n">
-        <v>-0.514343867902819</v>
+        <v>1.82059587713102</v>
       </c>
       <c r="S18" t="n">
-        <v>-0.52217738356536</v>
+        <v>-0.491676587343349</v>
       </c>
       <c r="T18" t="n">
-        <v>1.82059587713102</v>
+        <v>-0.458178581560971</v>
       </c>
       <c r="U18" t="n">
-        <v>-0.491676587343349</v>
-      </c>
-      <c r="V18" t="n">
-        <v>-0.458178581560971</v>
-      </c>
-      <c r="W18" t="n">
         <v>1.16119672402963</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="n">
-        <v>1.19267706091775</v>
+      <c r="A19" t="s">
+        <v>131</v>
       </c>
       <c r="B19" t="n">
         <v>-0.301052525341922</v>
       </c>
       <c r="C19" t="n">
-        <v>0.400086440006511</v>
+        <v>0.752966900840336</v>
       </c>
       <c r="D19" t="n">
-        <v>0.752966900840336</v>
+        <v>0.739135356142898</v>
       </c>
       <c r="E19" t="n">
-        <v>0.739135356142898</v>
+        <v>-1.07487700452682</v>
       </c>
       <c r="F19" t="n">
-        <v>-1.07487700452682</v>
+        <v>0.0975570138874772</v>
       </c>
       <c r="G19" t="n">
-        <v>0.0975570138874772</v>
+        <v>-0.0940086036329307</v>
       </c>
       <c r="H19" t="n">
-        <v>-0.0940086036329307</v>
+        <v>-0.295805526537364</v>
       </c>
       <c r="I19" t="n">
-        <v>-0.295805526537364</v>
+        <v>-0.298365811858222</v>
       </c>
       <c r="J19" t="n">
-        <v>-0.170151998725486</v>
+        <v>0.0659726205263397</v>
       </c>
       <c r="K19" t="n">
-        <v>-0.298365811858222</v>
+        <v>-0.680706980884602</v>
       </c>
       <c r="L19" t="n">
-        <v>0.0659726205263397</v>
+        <v>0.731435671047399</v>
       </c>
       <c r="M19" t="n">
-        <v>-0.680706980884602</v>
+        <v>-0.629644603624357</v>
       </c>
       <c r="N19" t="n">
-        <v>0.731435671047399</v>
+        <v>0.504763410749726</v>
       </c>
       <c r="O19" t="n">
-        <v>-0.629644603624357</v>
+        <v>1.19942050992602</v>
       </c>
       <c r="P19" t="n">
-        <v>0.504763410749726</v>
+        <v>0.764445140722727</v>
       </c>
       <c r="Q19" t="n">
-        <v>1.19942050992602</v>
+        <v>1.08579046865762</v>
       </c>
       <c r="R19" t="n">
-        <v>0.764445140722727</v>
+        <v>-0.364875457478697</v>
       </c>
       <c r="S19" t="n">
-        <v>1.08579046865762</v>
+        <v>0.529816936057543</v>
       </c>
       <c r="T19" t="n">
-        <v>-0.364875457478697</v>
+        <v>-0.138481719341181</v>
       </c>
       <c r="U19" t="n">
-        <v>0.529816936057543</v>
-      </c>
-      <c r="V19" t="n">
-        <v>-0.138481719341181</v>
-      </c>
-      <c r="W19" t="n">
         <v>-0.10087137914155</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="n">
-        <v>1.55915149151557</v>
+      <c r="A20" t="s">
+        <v>132</v>
       </c>
       <c r="B20" t="n">
         <v>1.51178286295268</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.766462374315664</v>
+        <v>-1.12500739453955</v>
       </c>
       <c r="D20" t="n">
-        <v>-1.12500739453955</v>
+        <v>-0.686614833628492</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.686614833628492</v>
+        <v>-0.793447341538777</v>
       </c>
       <c r="F20" t="n">
-        <v>-0.793447341538777</v>
+        <v>-0.503472638082524</v>
       </c>
       <c r="G20" t="n">
-        <v>-0.503472638082524</v>
+        <v>-0.901988217179735</v>
       </c>
       <c r="H20" t="n">
-        <v>-0.901988217179735</v>
+        <v>-0.316814936448309</v>
       </c>
       <c r="I20" t="n">
-        <v>-0.316814936448309</v>
+        <v>-1.01522515708039</v>
       </c>
       <c r="J20" t="n">
-        <v>-0.294968486980585</v>
+        <v>0.840194781016257</v>
       </c>
       <c r="K20" t="n">
-        <v>-1.01522515708039</v>
+        <v>-0.709857796440463</v>
       </c>
       <c r="L20" t="n">
-        <v>0.840194781016257</v>
+        <v>-0.408428270177506</v>
       </c>
       <c r="M20" t="n">
-        <v>-0.709857796440463</v>
+        <v>0.132602633438499</v>
       </c>
       <c r="N20" t="n">
-        <v>-0.408428270177506</v>
+        <v>-0.806939461985724</v>
       </c>
       <c r="O20" t="n">
-        <v>0.132602633438499</v>
+        <v>-0.234940129843345</v>
       </c>
       <c r="P20" t="n">
-        <v>-0.806939461985724</v>
+        <v>-0.275689548793253</v>
       </c>
       <c r="Q20" t="n">
-        <v>-0.234940129843345</v>
+        <v>-0.469835173122079</v>
       </c>
       <c r="R20" t="n">
-        <v>-0.275689548793253</v>
+        <v>0.646800454142474</v>
       </c>
       <c r="S20" t="n">
-        <v>-0.469835173122079</v>
+        <v>0.13496023829927</v>
       </c>
       <c r="T20" t="n">
-        <v>0.646800454142474</v>
+        <v>-0.194702699889872</v>
       </c>
       <c r="U20" t="n">
-        <v>0.13496023829927</v>
-      </c>
-      <c r="V20" t="n">
-        <v>-0.194702699889872</v>
-      </c>
-      <c r="W20" t="n">
         <v>0.931326995681454</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update patient and sample metadata tables and mutational signatures table to revised version
</commit_message>
<xml_diff>
--- a/tables/mutational_signatures.xlsx
+++ b/tables/mutational_signatures.xlsx
@@ -1782,7 +1782,7 @@
         <v>-2.62988386483926</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.37988467708953</v>
+        <v>-0.379884677089529</v>
       </c>
       <c r="L3" t="n">
         <v>-0.0875022228925386</v>
@@ -2011,7 +2011,7 @@
         <v>-0.337537440597022</v>
       </c>
       <c r="D5" t="n">
-        <v>0.903431994815011</v>
+        <v>0.903431994815012</v>
       </c>
       <c r="E5" t="n">
         <v>0.0889052030915567</v>
@@ -2276,7 +2276,7 @@
         <v>0.240234403215443</v>
       </c>
       <c r="I7" t="n">
-        <v>0.0004987546978926</v>
+        <v>0.00049875469789259</v>
       </c>
       <c r="J7" t="n">
         <v>-0.98873091217594</v>
@@ -2398,7 +2398,7 @@
         <v>0.631567978654499</v>
       </c>
       <c r="H8" t="n">
-        <v>-0.0025826772748678</v>
+        <v>-0.00258267727486779</v>
       </c>
       <c r="I8" t="n">
         <v>0.717114542961567</v>
@@ -2407,7 +2407,7 @@
         <v>-0.16544516494952</v>
       </c>
       <c r="K8" t="n">
-        <v>0.0520910653992999</v>
+        <v>0.0520910653992998</v>
       </c>
       <c r="L8" t="n">
         <v>0.137918645754952</v>
@@ -3092,7 +3092,7 @@
         <v>2.00598344354982</v>
       </c>
       <c r="AE13" t="n">
-        <v>-0.00757269751100255</v>
+        <v>-0.00757269751100254</v>
       </c>
       <c r="AF13" t="n">
         <v>-0.698556056875773</v>
@@ -3380,7 +3380,7 @@
         <v>111</v>
       </c>
       <c r="B16" t="n">
-        <v>0.426370365492864</v>
+        <v>0.426370365492865</v>
       </c>
       <c r="C16" t="n">
         <v>-0.856565852736064</v>
@@ -3565,7 +3565,7 @@
         <v>-0.217900097183202</v>
       </c>
       <c r="V17" t="n">
-        <v>-0.00199649232590794</v>
+        <v>-0.00199649232590793</v>
       </c>
       <c r="W17" t="n">
         <v>-0.152400432985517</v>

</xml_diff>